<commit_message>
refactoring and code clean up
</commit_message>
<xml_diff>
--- a/080A/ERSH_Discharging Plan_DARWIN_080A.xlsx
+++ b/080A/ERSH_Discharging Plan_DARWIN_080A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasat\Desktop\stowage-plan\080A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8428016E-5507-41D2-BD3A-D494A91CFE7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEDFF6-7C6B-4C1C-9D81-B43C01673950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E40F4C25-5628-4EF7-AE9B-E42FB112C086}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85ADBC91-F8FE-4798-A86A-FE3ECEF41EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Discharging Plan" sheetId="2" r:id="rId1"/>
@@ -227,13 +227,13 @@
     <t>PKL</t>
   </si>
   <si>
-    <t>MELBOURNE</t>
+    <t>MERLBOURNE</t>
   </si>
   <si>
     <t>MEL</t>
   </si>
   <si>
-    <t>FREMANTLE</t>
+    <t>FREMENTLE</t>
   </si>
   <si>
     <t>FRE</t>
@@ -384,7 +384,7 @@
     <numFmt numFmtId="166" formatCode="0\ &quot;u/t&quot;"/>
     <numFmt numFmtId="167" formatCode="0.0\ \t"/>
     <numFmt numFmtId="168" formatCode="0&quot;U/s&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.0&quot;kt&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.0&quot;mt&quot;"/>
     <numFmt numFmtId="170" formatCode="0\ &quot;p'kgs&quot;"/>
   </numFmts>
   <fonts count="27">
@@ -2477,9 +2477,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2489,9 +2486,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="16" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2519,6 +2513,9 @@
     <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2526,6 +2523,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2908,9 +2908,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{675313BD-CFB5-4C83-A407-533589FFA771}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{2A790099-F027-4239-9430-C9C753EA28E0}"/>
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
-    <cellStyle name="Нормален 2" xfId="1" xr:uid="{5BCCC09E-CF71-4EDE-8113-C93ECA8D3F76}"/>
+    <cellStyle name="Нормален 2" xfId="1" xr:uid="{CD0C3946-BD88-400A-84C5-FD83F2C590FC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2945,7 +2945,7 @@
         <xdr:cNvPr id="2" name="STOWAGE_PLAN_DEFAULT_SHAPE_705477">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B2286D5-3E35-4CF6-8B65-870BF9CE5BEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB3B00D-62F8-4300-AB14-366031C64124}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2955,7 +2955,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14597902" y="25774650"/>
+          <a:off x="14588377" y="25774650"/>
           <a:ext cx="201707" cy="798979"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartCollate">
@@ -2994,7 +2994,7 @@
         <xdr:cNvPr id="3" name="STOWAGE_PLAN_DEFAULT_SHAPE_533371">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D083C7D3-FA98-4728-8876-51B6323B3131}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BDCDD9D-CFAB-4C53-B3DB-3D3AE1B6A99F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3004,7 +3004,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14575493" y="23541319"/>
+          <a:off x="14565968" y="23541319"/>
           <a:ext cx="201707" cy="800099"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartCollate">
@@ -3043,7 +3043,7 @@
         <xdr:cNvPr id="4" name="STOWAGE_PLAN_DEFAULT_SHAPE_579461">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1439CEB3-FFF2-42A5-8277-2A3B4F6C4941}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29F8030-1221-4389-A8DC-606413FC1E4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3053,7 +3053,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9678520" y="24541443"/>
+          <a:off x="9668995" y="24541443"/>
           <a:ext cx="402267" cy="211281"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
@@ -3092,7 +3092,7 @@
         <xdr:cNvPr id="5" name="STOWAGE_PLAN_DEFAULT_SHAPE_289534">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098782A7-C462-4A31-9C61-DE42051DD209}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A05E43D-4A19-4EB6-A9BF-2A5AC51F7B36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3102,7 +3102,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="9992790" y="24541443"/>
+          <a:off x="9983265" y="24541443"/>
           <a:ext cx="402267" cy="211281"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
@@ -3141,7 +3141,7 @@
         <xdr:cNvPr id="6" name="STOWAGE_PLAN_DEFAULT_SHAPE_301918">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCFDB307-7B04-4558-B057-A69B206A9110}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0376E9C-BCC6-45A5-97A2-37E037D56BE2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3151,7 +3151,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9712138" y="22309231"/>
+          <a:off x="9702613" y="22309231"/>
           <a:ext cx="402267" cy="211281"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
@@ -3190,7 +3190,7 @@
         <xdr:cNvPr id="7" name="STOWAGE_PLAN_DEFAULT_SHAPE_774663">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AE75475-5B49-442F-A693-09354EC8DBBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBD00250-AF8C-4C58-BB50-8AA413EBF00C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3200,7 +3200,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="10026408" y="22309231"/>
+          <a:off x="10016883" y="22309231"/>
           <a:ext cx="402267" cy="211281"/>
         </a:xfrm>
         <a:prstGeom prst="rtTriangle">
@@ -3239,7 +3239,7 @@
         <xdr:cNvPr id="8" name="STOWAGE_PLAN_DEFAULT_SHAPE_14017">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4C3C38-4EBA-4603-AAC5-405E0134AAF9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{653C30B9-36EB-42A5-84FA-95D43D41615D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3249,7 +3249,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6518462" y="28481430"/>
+          <a:off x="6508937" y="28481430"/>
           <a:ext cx="2039470" cy="2218803"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3294,7 +3294,7 @@
         <xdr:cNvPr id="9" name="STOWAGE_PLAN_DEFAULT_SHAPE_760648">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DADEBA4-96A5-4B62-9634-53DD24D69A95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6699600D-513B-47C4-A70B-48758A9D9606}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3304,7 +3304,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6529668" y="26229049"/>
+          <a:off x="6520143" y="26229049"/>
           <a:ext cx="2039470" cy="2218802"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3349,7 +3349,7 @@
         <xdr:cNvPr id="10" name="STOWAGE_PLAN_DEFAULT_SHAPE_814409">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5D91022-5490-4621-A2E6-7B7A02B4023B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95782BF-31B8-49A9-A159-D22286DD73C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3359,7 +3359,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6502774" y="23984510"/>
+          <a:off x="6493249" y="23984510"/>
           <a:ext cx="2039470" cy="2218803"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3404,7 +3404,7 @@
         <xdr:cNvPr id="11" name="STOWAGE_PLAN_DEFAULT_SHAPE_708967">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1B46017-CF70-45DF-A9E3-BF90054B9732}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B92E5EB0-368F-43A3-BFA5-49F11D8F1287}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3414,7 +3414,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11661962" y="28435486"/>
+          <a:off x="11652437" y="28435486"/>
           <a:ext cx="2039470" cy="2218802"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3459,7 +3459,7 @@
         <xdr:cNvPr id="12" name="STOWAGE_PLAN_DEFAULT_SHAPE_45349">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2B7D63D-C41D-417B-B716-1C8E6DC4C551}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7CE0BE1-7BF8-419B-87C3-1846E4A39564}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3469,7 +3469,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11650756" y="26263787"/>
+          <a:off x="11641231" y="26263787"/>
           <a:ext cx="2039470" cy="2218802"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3514,7 +3514,7 @@
         <xdr:cNvPr id="13" name="STOWAGE_PLAN_DEFAULT_SHAPE_413992">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3888B959-A2CB-4B47-946A-FE6FB161F53A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{419780F2-0E14-446F-B677-45BCE18E665C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3524,7 +3524,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11668685" y="24006922"/>
+          <a:off x="11659160" y="24006922"/>
           <a:ext cx="2039470" cy="2218803"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3569,7 +3569,7 @@
         <xdr:cNvPr id="14" name="STOWAGE_PLAN_DEFAULT_SHAPE_862534">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCE28BB2-D1DD-4DDF-868C-C108EF199DC9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{344820F5-068F-4152-8C99-4CCD0E315276}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3579,7 +3579,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6529667" y="21783675"/>
+          <a:off x="6520142" y="21783675"/>
           <a:ext cx="2039470" cy="2217681"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3624,7 +3624,7 @@
         <xdr:cNvPr id="15" name="STOWAGE_PLAN_DEFAULT_SHAPE_790401">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88AE482-36F9-4793-AF67-C126289E48BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8454582-BAD4-4829-BE81-D421725CCF7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3634,7 +3634,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11673167" y="21783676"/>
+          <a:off x="11663642" y="21783676"/>
           <a:ext cx="2039470" cy="2217681"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3679,7 +3679,7 @@
         <xdr:cNvPr id="16" name="STOWAGE_PLAN_DEFAULT_SHAPE_373499">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54E27209-A43F-418F-BA96-7779EF20EF91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12F348EC-4C29-4A8C-A6AB-77395BABD82C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3728,7 +3728,7 @@
         <xdr:cNvPr id="17" name="STOWAGE_PLAN_DEFAULT_SHAPE_961857">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35927052-1656-40B2-853C-60427B465AF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E7231-CE37-4493-AC39-011EABF2491D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3777,7 +3777,7 @@
         <xdr:cNvPr id="18" name="STOWAGE_PLAN_DEFAULT_SHAPE_871359">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F24861-E889-41D7-8E62-BB7C36707167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A85E10-1F7E-475A-A047-82267C40FCFE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3787,7 +3787,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="7269256" y="5202331"/>
+          <a:off x="7259731" y="5202331"/>
           <a:ext cx="2077925" cy="2217644"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3832,7 +3832,7 @@
         <xdr:cNvPr id="19" name="STOWAGE_PLAN_DEFAULT_SHAPE_56232">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B8204E9-204E-4C96-A6C2-C07C7C505BD4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F601D33-F813-481F-B7D6-D20192318191}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3842,7 +3842,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="7258049" y="7442388"/>
+          <a:off x="7248524" y="7442388"/>
           <a:ext cx="2077925" cy="2217643"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3894,7 +3894,7 @@
         <xdr:cNvPr id="20" name="STOWAGE_PLAN_DEFAULT_SHAPE_949462">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3359C6B-0E0B-4368-97F6-3CD0B5358104}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B0FB942-F7DB-4612-AD62-71BDBFB7FC86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3904,7 +3904,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="7280462" y="9647703"/>
+          <a:off x="7270937" y="9647703"/>
           <a:ext cx="2077925" cy="2217644"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3949,7 +3949,7 @@
         <xdr:cNvPr id="21" name="STOWAGE_PLAN_DEFAULT_SHAPE_363983">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F640D54B-6074-499F-B614-D5E3EDAB72D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B1C058-AEE9-4D95-B206-A1B863D776E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3959,7 +3959,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="6126256" y="11877675"/>
+          <a:off x="6116731" y="11877675"/>
           <a:ext cx="3209719" cy="4221256"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4004,7 +4004,7 @@
         <xdr:cNvPr id="22" name="STOWAGE_PLAN_DEFAULT_SHAPE_524816">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E930E9A-719E-4132-961C-3E6AA8CF5449}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{606B5DBC-C1FC-4DEB-B1AD-EE921506912D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4014,7 +4014,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="5567363" y="16098929"/>
+          <a:off x="5557838" y="16098929"/>
           <a:ext cx="3768612" cy="4926318"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4059,7 +4059,7 @@
         <xdr:cNvPr id="23" name="STOWAGE_PLAN_DEFAULT_SHAPE_767035">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA52F13C-949C-443D-BFF1-E4DC9BE764F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C529BC4-C22D-42B7-87A8-07ADA122C6EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4069,7 +4069,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="16222756" y="7419976"/>
+          <a:off x="16213231" y="7419976"/>
           <a:ext cx="2077925" cy="2216522"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4114,7 +4114,7 @@
         <xdr:cNvPr id="24" name="STOWAGE_PLAN_DEFAULT_SHAPE_53500">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C527A8EF-995C-4344-97D6-B18EFE787DB9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0825E04-7393-42E2-B0F8-EEA8C32BD1C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4124,7 +4124,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="14743580" y="9660029"/>
+          <a:off x="14734055" y="9660029"/>
           <a:ext cx="3742765" cy="4422963"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4169,7 +4169,7 @@
         <xdr:cNvPr id="25" name="STOWAGE_PLAN_DEFAULT_SHAPE_592400">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CF30F56-EE8A-4F75-A9E8-14C61224A86A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6959C169-2B04-437F-BD1B-284E07D7A637}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4179,7 +4179,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="11449050" y="14128936"/>
+          <a:off x="11439525" y="14128936"/>
           <a:ext cx="2279632" cy="2194112"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4224,7 +4224,7 @@
         <xdr:cNvPr id="26" name="STOWAGE_PLAN_DEFAULT_SHAPE_468654">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE90668-BD95-45FC-B8AF-3D22DAFBE44F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF6B8123-477E-4C10-A6F2-C2040DED0064}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4234,7 +4234,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="11493874" y="16346581"/>
+          <a:off x="11484349" y="16346581"/>
           <a:ext cx="3758807" cy="4670610"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -4279,7 +4279,7 @@
         <xdr:cNvPr id="27" name="STOWAGE_PLAN_DEFAULT_SHAPE_298136">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{118946C2-78F8-4920-BE5B-94C7BA96CE62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9382D690-D1CE-43E8-BBBF-F617072B4EFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4329,7 +4329,7 @@
         <xdr:cNvPr id="28" name="PKG_BOX_20201019110448_PKGS">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CC2A44-DDCA-4399-8C6B-B01C1B403FEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89331310-9844-4E5C-876E-88E59608F14C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4415,7 +4415,7 @@
         <xdr:cNvPr id="29" name="STOWAGE_PLAN_DEFAULT_SHAPE_622635">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA62B6C8-AC9F-45DF-8444-B4A4786125AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{130A0BD3-2107-41CB-9620-1EA932E7B8C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4424,7 +4424,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063511" y="30925318"/>
-          <a:ext cx="2142478" cy="529663"/>
+          <a:ext cx="2132953" cy="529663"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4537,7 +4537,7 @@
         <xdr:cNvPr id="30" name="STOWAGE_PLAN_DEFAULT_SHAPE_829719">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC93B41E-825C-479B-8DBF-5B40F2E8C580}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA949FA-EF4F-460E-8E78-77595325E601}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4586,7 +4586,7 @@
         <xdr:cNvPr id="31" name="STOWAGE_PLAN_DEFAULT_SHAPE_824520">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F69BA062-6797-44EE-8695-18FE5277CCCD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57581CDE-D94B-4248-AC21-DF7B3B1A42F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4657,7 +4657,7 @@
         <xdr:cNvPr id="32" name="STOWAGE_PLAN_DEFAULT_SHAPE_589105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EFA891B-D8D9-470D-B612-4B2B6BC7D946}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA2078DF-AF93-4D42-9132-B151A0C319BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4723,7 +4723,7 @@
         <xdr:cNvPr id="33" name="STOWAGE_PLAN_DEFAULT_SHAPE_985995">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFE8DF90-4504-46C6-9ACB-E89660EC8E5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D446AE8-BB6F-42E4-9795-2DF75A82D927}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4732,7 +4732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2067572" y="24060745"/>
-          <a:ext cx="2142478" cy="531282"/>
+          <a:ext cx="2132953" cy="531282"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4836,7 +4836,7 @@
         <xdr:cNvPr id="34" name="STOWAGE_PLAN_DEFAULT_SHAPE_910874">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B523F6-0796-44F0-89A7-B9A3E4FB77F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93DA598C-7D4F-4DAF-B851-C685C622A83E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4902,7 +4902,7 @@
         <xdr:cNvPr id="35" name="STOWAGE_PLAN_DEFAULT_SHAPE_226844">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8253297C-682C-4DFC-A2AD-8D83DD6D3988}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8DCA4CB-CEF7-41EB-ABD2-1C71E49737C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4911,7 +4911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2067572" y="24592027"/>
-          <a:ext cx="2142478" cy="528976"/>
+          <a:ext cx="2132953" cy="528976"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5015,7 +5015,7 @@
         <xdr:cNvPr id="36" name="STOWAGE_PLAN_DEFAULT_SHAPE_695046">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{520945D1-520A-47A3-B658-6E85752EBFAA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E005E2D1-173E-40AF-9446-80C37594A367}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5081,7 +5081,7 @@
         <xdr:cNvPr id="37" name="STOWAGE_PLAN_DEFAULT_SHAPE_979906">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BDEB7D5-EBED-468B-9D6B-5E68874D6EA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71C04812-10F7-4BD0-96B4-27754506D307}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5090,7 +5090,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2067572" y="25121004"/>
-          <a:ext cx="2142478" cy="531282"/>
+          <a:ext cx="2132953" cy="531282"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5182,7 +5182,7 @@
         <xdr:cNvPr id="38" name="STOWAGE_PLAN_DEFAULT_SHAPE_243907">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B02C2EF-D1EF-480A-BE13-C0BF71DDE32A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{635BCF5B-FE90-4137-81C9-AAC445F598F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5248,7 +5248,7 @@
         <xdr:cNvPr id="39" name="STOWAGE_PLAN_DEFAULT_SHAPE_533820">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DE14CE6-2BD1-4DB8-810C-81C2FA0D73AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DDB2E1C-5731-40BB-B6D7-DA8E1B43677A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5257,7 +5257,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2065753" y="26714018"/>
-          <a:ext cx="2142478" cy="533210"/>
+          <a:ext cx="2132953" cy="533210"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5376,7 +5376,7 @@
         <xdr:cNvPr id="40" name="STOWAGE_PLAN_DEFAULT_SHAPE_106360">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061EFE22-C7AA-4D4E-B9FE-FAFB2F2B00C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A379AB30-55CC-46F0-B6DC-BEF4B52AB129}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5442,7 +5442,7 @@
         <xdr:cNvPr id="41" name="STOWAGE_PLAN_DEFAULT_SHAPE_999315">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5984643F-2B2D-4CB7-A889-3583CA4864C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F1CEFE-A716-4F1F-B8D6-7432366991ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5451,7 +5451,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063512" y="27767164"/>
-          <a:ext cx="2142478" cy="533315"/>
+          <a:ext cx="2132953" cy="533315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5543,7 +5543,7 @@
         <xdr:cNvPr id="42" name="STOWAGE_PLAN_DEFAULT_SHAPE_676109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6131890-626D-46DC-99C5-957022BBC774}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{649FF446-D07C-400A-81E3-F027DB929E36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5609,7 +5609,7 @@
         <xdr:cNvPr id="43" name="STOWAGE_PLAN_DEFAULT_SHAPE_15703">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{424F5DA2-3248-4763-90E0-6D761D68547C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EC036DE-1551-4D52-B140-911614FEE5B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5618,7 +5618,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063512" y="28300480"/>
-          <a:ext cx="2142478" cy="526942"/>
+          <a:ext cx="2132953" cy="526942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5710,7 +5710,7 @@
         <xdr:cNvPr id="44" name="STOWAGE_PLAN_DEFAULT_SHAPE_575127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF6E8BE4-78BF-4DDE-B86E-C207C13E693F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E4B994-1437-47B2-8D2C-95E85DAACC6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5764,7 +5764,7 @@
         <xdr:cNvPr id="45" name="STOWAGE_PLAN_DEFAULT_SHAPE_100043">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AB45392-3D53-4220-9A5F-24F55A085386}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48B70C4-BC76-4235-BEFE-E3CCCB4993F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5818,7 +5818,7 @@
         <xdr:cNvPr id="46" name="STOWAGE_PLAN_DEFAULT_SHAPE_103013">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34CD7E38-0CA1-4C34-9F05-9964441D2F3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5649D2E-FA4A-4F88-BE87-48429F927B0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5869,7 +5869,7 @@
         <xdr:cNvPr id="47" name="STOWAGE_PLAN_DEFAULT_SHAPE_798805">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3FEB164-91A0-422B-91C4-AA34AB5417CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44CF477-1AC0-44ED-A6F7-96284D1153CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5920,7 +5920,7 @@
         <xdr:cNvPr id="48" name="STOWAGE_PLAN_DEFAULT_SHAPE_284452">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC6D623-1C08-402F-8A03-D5347C07CD0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B943B497-9CBB-4144-A336-DC2E8472B12C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5969,7 +5969,7 @@
         <xdr:cNvPr id="49" name="STOWAGE_PLAN_DEFAULT_SHAPE_45645">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA108C38-655C-4177-ABAC-18F1797BBF82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E99AD3DD-06B8-40E2-887A-F52D8E98D225}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6018,7 +6018,7 @@
         <xdr:cNvPr id="50" name="STOWAGE_PLAN_DEFAULT_SHAPE_295744">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112F9D9E-B5EA-4D9C-B916-51FE9ABF02A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E8A6509-09C3-47D7-87E7-F1A3C4C82A84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6084,7 +6084,7 @@
         <xdr:cNvPr id="51" name="STOWAGE_PLAN_DEFAULT_SHAPE_381973">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCEA5188-BB9E-43BD-BC3D-BF45AB0BA3C9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B19DFD27-7968-46AF-8B91-ED73B13F7A8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6093,7 +6093,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2064238" y="26180969"/>
-          <a:ext cx="2145811" cy="528350"/>
+          <a:ext cx="2136286" cy="528350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6185,7 +6185,7 @@
         <xdr:cNvPr id="52" name="STOWAGE_PLAN_DEFAULT_SHAPE_300941">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3E1919-9633-4758-A4C6-5C445C1660D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E388CBEC-ADEF-4882-BC2D-6665EF3BDF6B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6251,7 +6251,7 @@
         <xdr:cNvPr id="53" name="STOWAGE_PLAN_DEFAULT_SHAPE_948477">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB19BEB2-BB0A-4931-9F06-C162D1DA39BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFDDD0A-CDAC-4120-A060-C30EF8092734}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6260,7 +6260,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063512" y="29354470"/>
-          <a:ext cx="2142478" cy="526941"/>
+          <a:ext cx="2132953" cy="526941"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6352,7 +6352,7 @@
         <xdr:cNvPr id="54" name="STOWAGE_PLAN_DEFAULT_SHAPE_979732">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98B7F357-FAC5-4E1E-9FCB-7091D8491EB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{754AA272-8262-4858-834D-AA9FC745D073}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6407,7 +6407,7 @@
         <xdr:cNvPr id="55" name="STOWAGE_PLAN_DEFAULT_SHAPE_401335">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7504E8FF-1F46-464E-9DC2-37E76EAE2579}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C57615CA-5434-41BB-83A2-6012E10C5B6F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6473,7 +6473,7 @@
         <xdr:cNvPr id="56" name="STOWAGE_PLAN_DEFAULT_SHAPE_278253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F92FC6F-035C-4A73-A575-55146F21FEB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FFB43E4-7CF4-4830-873B-D7B894609782}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6482,7 +6482,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063512" y="29878224"/>
-          <a:ext cx="2142478" cy="526942"/>
+          <a:ext cx="2132953" cy="526942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6573,7 +6573,7 @@
         <xdr:cNvPr id="57" name="STOWAGE_PLAN_DEFAULT_SHAPE_160426">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B037C6AB-E082-46D0-879A-309038C4B4B1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DBBDBAB-9880-4797-9A7C-D5AA6AAF2336}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6640,7 +6640,7 @@
         <xdr:cNvPr id="58" name="STOWAGE_PLAN_DEFAULT_SHAPE_162806">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BC3FC24-1548-4DF0-9C36-1E10CAD078D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDF0B058-E2BE-4A2E-8AB5-6DB27A0CAEC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6706,7 +6706,7 @@
         <xdr:cNvPr id="59" name="STOWAGE_PLAN_DEFAULT_SHAPE_646523">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6DD7D8B-0F58-479B-9E91-C34C482CA05D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80FF802B-42C6-4CE2-8237-1EDB06B11F91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6715,7 +6715,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2063512" y="30401771"/>
-          <a:ext cx="2142478" cy="526942"/>
+          <a:ext cx="2132953" cy="526942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6828,7 +6828,7 @@
         <xdr:cNvPr id="60" name="STOWAGE_PLAN_DEFAULT_SHAPE_410033">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A492D912-CB29-4000-8244-808DF72EB3B8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53397A9C-8106-4838-9DAA-F05189B7A77C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6894,7 +6894,7 @@
         <xdr:cNvPr id="61" name="STOWAGE_PLAN_DEFAULT_SHAPE_412726">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D92B4BB5-E371-4301-9BC9-8D46DF9D97EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EADCA3D2-1C0B-44C2-BC96-690E89564C54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6988,7 +6988,7 @@
         <xdr:cNvPr id="62" name="STOWAGE_PLAN_DEFAULT_SHAPE_712660">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD5F03F8-5E3B-4429-8797-191E555E36C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5F5FE8-9D23-4E41-B6CA-411D5FEE3C97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7044,7 +7044,7 @@
         <xdr:cNvPr id="63" name="STOWAGE_PLAN_DEFAULT_SHAPE_326174">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D26FD7B1-54B6-4961-91FB-96E77EE548F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{691A7FAC-6F39-4043-BACA-89F9E7BE4F0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7100,7 +7100,7 @@
         <xdr:cNvPr id="64" name="STOWAGE_PLAN_DEFAULT_SHAPE_633116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9D2D666-00EA-405B-A9BD-921C1526D407}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{300148E3-4432-4E02-B213-08BD213CB07E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7156,7 +7156,7 @@
         <xdr:cNvPr id="65" name="STOW_DIRECTION_20201021231228_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AAA8101-9A42-4901-AD62-729B56C81ABA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0927A168-63F6-4359-8205-3C5BAD0DF002}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7165,7 +7165,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="3134285" y="5697632"/>
-          <a:ext cx="1270001" cy="190498"/>
+          <a:ext cx="1260476" cy="190498"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7236,7 +7236,7 @@
         <xdr:cNvPr id="66" name="STOW_DIRECTION_20201021231242_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{112FC528-E29F-4908-8211-718F9F1C8774}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD0030E1-2FAD-44D8-93FA-C60D47B828FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7245,7 +7245,7 @@
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
           <a:off x="3235137" y="4234141"/>
-          <a:ext cx="1270001" cy="176679"/>
+          <a:ext cx="1260476" cy="176679"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7316,7 +7316,7 @@
         <xdr:cNvPr id="67" name="STOW_DIRECTION_20201021231253_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0169BE-D36A-4DA0-9570-4719930D40AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433387B3-B241-494B-8D4D-BB80C7573027}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7396,7 +7396,7 @@
         <xdr:cNvPr id="68" name="STOW_DIRECTION_20201021231242_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11ACF204-3400-432A-96E7-1EDBC5F0FA30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{061FE543-372E-4F3D-97AA-847A060F73C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7404,7 +7404,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7057390" y="4208145"/>
+          <a:off x="7047865" y="4208145"/>
           <a:ext cx="1280160" cy="182880"/>
         </a:xfrm>
         <a:custGeom>
@@ -7476,7 +7476,7 @@
         <xdr:cNvPr id="69" name="STOW_DIRECTION_20201021231228_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50585B36-ABCD-4953-97A5-B7B1D97AABF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E58EBB81-D977-4910-9DDC-F3BC6A9899C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7484,7 +7484,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6899463" y="5753661"/>
+          <a:off x="6889938" y="5753661"/>
           <a:ext cx="1270001" cy="191619"/>
         </a:xfrm>
         <a:custGeom>
@@ -7556,7 +7556,7 @@
         <xdr:cNvPr id="70" name="STOW_DIRECTION_20201021231712_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2439C370-6A71-4E2D-9AB1-79113958F86C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51D31C15-3807-4B77-AEED-AE7CD8B92F9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7564,7 +7564,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="-5400000" flipV="1">
-          <a:off x="9554696" y="5572683"/>
+          <a:off x="9545171" y="5572683"/>
           <a:ext cx="751915" cy="168092"/>
         </a:xfrm>
         <a:custGeom>
@@ -7636,7 +7636,7 @@
         <xdr:cNvPr id="71" name="STOW_DIRECTION_20201021231727_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B8BFFB-BB46-43DF-A8F9-7EDB5236F7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E39A9067-E4DA-4773-8357-9237EBC5FDD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7644,7 +7644,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="9510430" y="4807884"/>
+          <a:off x="9500905" y="4807884"/>
           <a:ext cx="694765" cy="135592"/>
         </a:xfrm>
         <a:custGeom>
@@ -7716,7 +7716,7 @@
         <xdr:cNvPr id="72" name="STOW_DIRECTION_20201021231242_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C3B1FAB-EF25-480F-9ABA-5A3169D52772}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{913EC9C9-F896-4ABA-B0DC-B1EB10116C5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7724,7 +7724,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="10911167" y="5720042"/>
+          <a:off x="10901642" y="5720042"/>
           <a:ext cx="1280160" cy="182880"/>
         </a:xfrm>
         <a:custGeom>
@@ -7796,7 +7796,7 @@
         <xdr:cNvPr id="73" name="STOW_DIRECTION_20201021231242_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2C4A8F-EA4E-4BE5-9D0C-93C30FAE5161}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886505F2-4FC2-409D-AD05-96F866E81EAE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7804,7 +7804,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="10933579" y="4256554"/>
+          <a:off x="10924054" y="4256554"/>
           <a:ext cx="1280160" cy="182880"/>
         </a:xfrm>
         <a:custGeom>
@@ -7876,7 +7876,7 @@
         <xdr:cNvPr id="74" name="STOW_DIRECTION_20201021231242_DRW">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{750D9965-4EB8-46BB-81AF-A694D821B18F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA2B5E7-E2B5-4F60-9114-27CD7DF7A1F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7884,7 +7884,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="12311903" y="4977093"/>
+          <a:off x="12302378" y="4977093"/>
           <a:ext cx="1280160" cy="182880"/>
         </a:xfrm>
         <a:custGeom>
@@ -7956,7 +7956,7 @@
         <xdr:cNvPr id="75" name="STOWAGE_PLAN_DEFAULT_SHAPE_583301">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E62161F4-B16C-48F1-95BC-5E6C43234924}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E28E6DA0-9291-4B62-A122-9D76C715C142}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8032,22 +8032,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
+      <xdr:colOff>145676</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>201706</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
+      <xdr:colOff>145676</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>19023</xdr:rowOff>
+      <xdr:rowOff>7817</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="76" name="STOWAGE_PLAN_DEFAULT_SHAPE_80707">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95944DAA-72F4-4473-80BF-1BC1B1D2D2CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{686A5859-5071-4675-AC22-88906986E12A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8055,7 +8055,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5162549" y="5392831"/>
+          <a:off x="5108201" y="5381625"/>
           <a:ext cx="1524000" cy="312617"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8138,7 +8138,7 @@
         <xdr:cNvPr id="77" name="STOWAGE_PLAN_DEFAULT_SHAPE_457926">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD69AEB9-5D88-4403-9C0B-3CC9DC7B5407}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89E36DA9-F73D-4EB1-B908-3B8B3C8E7212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8146,7 +8146,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10754285" y="5461187"/>
+          <a:off x="10744760" y="5461187"/>
           <a:ext cx="1524000" cy="311496"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8229,7 +8229,7 @@
         <xdr:cNvPr id="78" name="STOWAGE_PLAN_DEFAULT_SHAPE_905640">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{531F78E9-6339-4486-BC72-0870E64D0A86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{372163A3-E43E-4A23-9BDC-7D651DF3BE45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8295,7 +8295,7 @@
         <xdr:cNvPr id="79" name="STOWAGE_PLAN_DEFAULT_SHAPE_261343">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92CD68CC-C7B5-4592-85A6-C7191FE8DCB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{333C3EE2-E1F6-445A-99EC-A03A3F3EDD8E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8304,7 +8304,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2064757" y="28826795"/>
-          <a:ext cx="2142478" cy="526942"/>
+          <a:ext cx="2132953" cy="526942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8408,7 +8408,7 @@
         <xdr:cNvPr id="80" name="STOWAGE_PLAN_DEFAULT_SHAPE_785134">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C8CA85-BE48-4430-B41F-BDDC997FDF6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69B4C930-4AF7-4E01-9B70-E6194E5B0804}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8463,7 +8463,7 @@
         <xdr:cNvPr id="81" name="STOWAGE_PLAN_DEFAULT_SHAPE_378865">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0941F6D2-2446-4115-966E-BDB09133E2B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFF1B432-E179-4532-9824-C6DD5EBFC380}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8529,7 +8529,7 @@
         <xdr:cNvPr id="82" name="STOWAGE_PLAN_DEFAULT_SHAPE_289637">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{664020FA-749D-4574-BB09-6899EC77F525}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713F4076-6E53-41F9-A93B-7870D74EE52E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8538,7 +8538,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2070614" y="27238958"/>
-          <a:ext cx="2140058" cy="528977"/>
+          <a:ext cx="2130533" cy="528977"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8657,7 +8657,7 @@
         <xdr:cNvPr id="83" name="STOWAGE_PLAN_DEFAULT_SHAPE_919286">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D448BF7-20F5-4006-A67B-33F6A5DA44AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE723293-99FB-473E-ACC3-95007C2AFD14}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8708,7 +8708,7 @@
         <xdr:cNvPr id="84" name="STOWAGE_PLAN_DEFAULT_SHAPE_631680">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB2EFD2-828E-45EB-A507-0EE0597BD93A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE77C93B-4365-417A-81F1-9719969803C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8774,7 +8774,7 @@
         <xdr:cNvPr id="85" name="STOWAGE_PLAN_DEFAULT_SHAPE_627580">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FEB18D8-23E6-4A78-8F9C-4F230DD092A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD7E0B5-040A-43AF-B2FD-3D8A58BE5685}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8783,7 +8783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2072433" y="25652283"/>
-          <a:ext cx="2142478" cy="531281"/>
+          <a:ext cx="2132953" cy="531281"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8875,7 +8875,7 @@
         <xdr:cNvPr id="86" name="STOWAGE_PLAN_DEFAULT_SHAPE_428414">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{340DA477-AC9C-4682-8882-96B36EB6E807}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00455BD1-5CEC-404C-B939-3E58B022783E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8941,7 +8941,7 @@
         <xdr:cNvPr id="87" name="STOWAGE_PLAN_DEFAULT_SHAPE_560984">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74CA150B-65AB-4B3C-9A4C-9A992D684D78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D30D24-67CC-424A-9E99-5FE948D437C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8951,7 +8951,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8903851" y="20741285"/>
+          <a:off x="8894326" y="20741285"/>
           <a:ext cx="787294" cy="211204"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9020,7 +9020,7 @@
         <xdr:cNvPr id="88" name="STOWAGE_PLAN_DEFAULT_SHAPE_694416">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B5B8D5-FE80-4FBA-99E8-92B6EC2FC054}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09B5C96-E8E2-4D3C-8942-2880ED30B1D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9030,7 +9030,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="5555457" y="18316575"/>
+          <a:off x="5545932" y="18316575"/>
           <a:ext cx="3798093" cy="2730103"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9075,7 +9075,7 @@
         <xdr:cNvPr id="89" name="STOWAGE_PLAN_DEFAULT_SHAPE_913627">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CFC0819-634C-4116-82F4-9AD2EE521C01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F441E5D8-E444-4183-AED9-784A7DD5E027}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9083,7 +9083,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6162675" y="20311694"/>
+          <a:off x="6153150" y="20311694"/>
           <a:ext cx="171450" cy="137748"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -9132,7 +9132,7 @@
         <xdr:cNvPr id="90" name="STOWAGE_PLAN_DEFAULT_SHAPE_834734">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36D9B4D3-B988-4A4E-8D71-40AF956971BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95F9B4C-2D20-4B95-AC4B-B663EA78B2F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9142,7 +9142,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="11456377" y="18571551"/>
+          <a:off x="11446852" y="18571551"/>
           <a:ext cx="3788019" cy="2461938"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9187,7 +9187,7 @@
         <xdr:cNvPr id="91" name="STOWAGE_PLAN_DEFAULT_SHAPE_22627">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A50CD85-85A4-4049-B874-6066963E7BE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D155D01-86A1-4DA8-BF68-000A870163AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9195,7 +9195,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12087225" y="20318290"/>
+          <a:off x="12077700" y="20318290"/>
           <a:ext cx="152400" cy="179510"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -9244,7 +9244,7 @@
         <xdr:cNvPr id="92" name="STOWAGE_PLAN_DEFAULT_SHAPE_543307">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA2AB148-E31C-4834-9BF8-26BB0120FFAE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6538E7C7-8948-43A4-B96B-6C618B086B00}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9254,7 +9254,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="6137463" y="14117730"/>
+          <a:off x="6127938" y="14117730"/>
           <a:ext cx="3216088" cy="1963620"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9299,7 +9299,7 @@
         <xdr:cNvPr id="93" name="STOWAGE_PLAN_DEFAULT_SHAPE_916073">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB8EB18-DCBB-453D-B10F-4A6838458F86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B16E689D-C6F6-4E37-80B7-47A745008CA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9307,7 +9307,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14912286" y="13675593"/>
+          <a:off x="14902761" y="13675593"/>
           <a:ext cx="265530" cy="181881"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -9356,7 +9356,7 @@
         <xdr:cNvPr id="94" name="STOWAGE_PLAN_DEFAULT_SHAPE_430219">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0AAE8DB-6DD3-47CF-AFFA-AF088D5BD007}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{800B3704-1170-466E-8084-FD5413CE0BE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9366,7 +9366,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="14743579" y="11845373"/>
+          <a:off x="14734054" y="11845373"/>
           <a:ext cx="2395623" cy="2243572"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -9411,7 +9411,7 @@
         <xdr:cNvPr id="95" name="STOWAGE_PLAN_DEFAULT_SHAPE_677880">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{754081F1-2B95-46EA-814B-6A32CC09DE67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC97285-3D7B-4FED-8403-B104C8475B76}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9419,7 +9419,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6562725" y="15554325"/>
+          <a:off x="6553200" y="15554325"/>
           <a:ext cx="182440" cy="184638"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -9468,7 +9468,7 @@
         <xdr:cNvPr id="96" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{073353EF-6042-4118-ABDD-1094B3312404}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA6CF602-A3A5-497F-8F0F-67E21E239D99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9553,7 +9553,7 @@
         <xdr:cNvPr id="97" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC8C615-5342-4269-AF31-5C1709BC6C34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847F25F0-A9F7-42BF-B46E-576CBA6511E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9619,7 +9619,7 @@
         <xdr:cNvPr id="98" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD5A39B2-2F10-4937-BADE-447F372CE500}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA5A78F-02E4-4C3E-B62E-D1437FB6204C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9685,7 +9685,7 @@
         <xdr:cNvPr id="99" name="STOWAGE_PLAN_DEFAULT_SHAPE_428414">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B4359B6-DD22-46AB-AEA8-366F7FE45C35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{904F80A2-5D34-4B08-BB76-D4661195F4D1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9695,7 +9695,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7295427" y="20587025"/>
+          <a:off x="7285902" y="20587025"/>
           <a:ext cx="332417" cy="182518"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9751,7 +9751,7 @@
         <xdr:cNvPr id="100" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{644A6547-2CEC-4729-9B5C-8392AD2757D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB29B96D-F6F4-4E8B-AE53-001162C2762F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9761,7 +9761,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7291668" y="20331393"/>
+          <a:off x="7282143" y="20331393"/>
           <a:ext cx="471621" cy="252036"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9801,23 +9801,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>145677</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>44822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>59</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>156880</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="101" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FC7CE58-8687-4ED8-AC35-6F95A3395BD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4107180F-6EA7-42CE-93E6-F6883360BAF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9827,8 +9827,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10563785" y="16864293"/>
-          <a:ext cx="885265" cy="370912"/>
+          <a:off x="7775202" y="20342597"/>
+          <a:ext cx="829235" cy="370917"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9883,7 +9883,7 @@
         <xdr:cNvPr id="102" name="STOW_DIRECTION_20201026082459_FRE">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C3C265-E1D6-41F9-B3F5-C63E89298775}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98603C25-EC22-4024-BE92-F9F2AEDC3271}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9891,7 +9891,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3593727" y="8027334"/>
+          <a:off x="3584202" y="8027334"/>
           <a:ext cx="1270001" cy="146797"/>
         </a:xfrm>
         <a:custGeom>
@@ -9947,99 +9947,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>64620</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>239835</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>64620</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>212612</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="103" name="PKG_BOX_20201026232230_PKGS">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B9ABD85-B951-4814-B52F-36E680F87EDE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9418170" y="6421560"/>
-          <a:ext cx="1524000" cy="468077"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -25980"/>
-            <a:gd name="adj2" fmla="val -180460"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="99CCFF">
-            <a:alpha val="90000"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr" anchorCtr="1">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DRW / LCH</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>12 pkgs - 23.0 kt</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>189379</xdr:colOff>
       <xdr:row>38</xdr:row>
@@ -10053,10 +9960,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="PKG_BOX_20201026232900_PKGS">
+        <xdr:cNvPr id="103" name="PKG_BOX_20201026232900_PKGS">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE9EEDE7-006F-48F0-AEEA-A652F661E641}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2F8D9A1-6BA0-4840-A77E-805EA8511150}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10121,7 +10028,7 @@
                 <a:srgbClr val="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>23 pkgs - 44.0 kt</a:t>
+            <a:t>33 pkgs - 44.0 kt</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -10130,23 +10037,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>206568</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>64620</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>139334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>165941</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>64620</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>98707</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="105" name="PKG_BOX_20201027052509_PKGS">
+        <xdr:cNvPr id="104" name="PKG_BOX_20201027052509_PKGS">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A208F1AE-5ED6-4063-81F2-79646580978C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D79E29AE-6734-4FBE-B69C-37A8F34C4078}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10154,13 +10061,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4902200" y="3664143"/>
+          <a:off x="4646145" y="3349259"/>
           <a:ext cx="1524000" cy="454673"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -17157"/>
-            <a:gd name="adj2" fmla="val 115422"/>
+            <a:gd name="adj1" fmla="val -1716"/>
+            <a:gd name="adj2" fmla="val 179819"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -10254,7 +10161,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>12 pkgs  - 25.5 kt</a:t>
+            <a:t> 12 pkgs - 12.5 kt  </a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1200">
             <a:solidFill>
@@ -10268,23 +10175,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>206217</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>30507</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>178994</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>94353</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="PKG_BOX_20201028080211_PKGS">
+        <xdr:cNvPr id="105" name="20201030034148_DRW_INFO">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E163E04-3D54-491C-B10D-9C9F9AA6899B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFAE4CE-6A05-4EA9-A09A-D7E7E9431C7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10292,22 +10199,34 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9093200" y="3911442"/>
-          <a:ext cx="1524000" cy="468077"/>
+          <a:off x="3200400" y="4231032"/>
+          <a:ext cx="1514475" cy="311496"/>
         </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
           <a:srgbClr val="99CCFF">
-            <a:alpha val="90000"/>
+            <a:alpha val="0"/>
           </a:srgbClr>
         </a:solidFill>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -10332,25 +10251,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>DRW / LCH</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1200">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>3 pkgs - 434.0 kt</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10379,7 +10284,7 @@
         <xdr:cNvPr id="2" name="STOWAGE_PLAN_DEFAULT_SHAPE_502404" descr="DK5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1244E873-E0D8-4B83-A4AA-4B259B29FBC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{332A2F2B-B68D-4E99-8702-286CF2A37043}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10451,7 +10356,7 @@
         <xdr:cNvPr id="3" name="STOWAGE_PLAN_DEFAULT_SHAPE_513687">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666F0570-5241-451B-B036-4CA60C0C75CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D499A9CC-C04A-464C-B265-8F01752C35A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10567,7 +10472,7 @@
         <xdr:cNvPr id="4" name="PKG_BOX_20201019110441_PKGS">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F1287F-D221-41D4-8B95-4FA84EDE08E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D8C1EC-6E37-43E6-90F9-8FA0AC977C0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10649,7 +10554,7 @@
         <xdr:cNvPr id="5" name="STOWAGE_PLAN_DEFAULT_SHAPE_404794">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A63D888-3D48-4B94-AAA4-36D6CAF81226}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1EEC44-1A1D-4528-AD37-FFC35544D30A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10732,7 +10637,7 @@
         <xdr:cNvPr id="6" name="STOWAGE_PLAN_DEFAULT_SHAPE_269705">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F7E39A2-7A55-4EFC-995A-038C14E3A81A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C50E3062-FEC5-429B-A3DC-CFA637BB6397}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10815,7 +10720,7 @@
         <xdr:cNvPr id="7" name="STOWAGE_PLAN_DEFAULT_SHAPE_55588">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DEAFFE8-43F2-4164-824A-AA26596723C0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B050F90D-BE48-471F-B633-C7B00EA95A4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10892,7 +10797,7 @@
         <xdr:cNvPr id="8" name="STOWAGE_PLAN_DEFAULT_SHAPE_243821">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A7C77E1-21D7-4F73-984A-8DD015F58C27}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE3E9BD-1713-423D-9FE0-16F914A93730}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10941,7 +10846,7 @@
         <xdr:cNvPr id="9" name="STOWAGE_PLAN_DEFAULT_SHAPE_978981">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C91EBD1-1861-4F8F-A8CB-913B95A852AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C595A4AF-8F40-4EFF-8BE5-91EA19B128C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11012,7 +10917,7 @@
         <xdr:cNvPr id="10" name="STOWAGE_PLAN_DEFAULT_SHAPE_390253">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAAE309C-1BD9-4264-8AA0-B20E400A4E0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A96AA116-8397-4308-8FDE-8B3AAF54E636}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11061,7 +10966,7 @@
         <xdr:cNvPr id="11" name="STOWAGE_PLAN_DEFAULT_SHAPE_364959">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB24D01D-660F-40D2-971E-E7B0A6405C06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D0F4778-E9E9-4BEB-945E-FD22564449A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11146,7 +11051,7 @@
         <xdr:cNvPr id="12" name="STOWAGE_PLAN_DEFAULT_SHAPE_474412">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A804A4D-BE88-4412-BE8E-2447EB79B137}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{445DAC78-1A74-477C-BF75-60591D2495AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11201,7 +11106,7 @@
         <xdr:cNvPr id="13" name="STOWAGE_PLAN_DEFAULT_SHAPE_257242">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9A4782A-8DC9-432E-B499-AA8D5F2AAF9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A707958-B82F-4753-AF77-352C3EE35250}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11256,7 +11161,7 @@
         <xdr:cNvPr id="14" name="STOWAGE_PLAN_DEFAULT_SHAPE_628689">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1FA26C8-87BE-4F87-9C52-7A5B27F3B55E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A238D3CF-811A-405D-8420-304A34BAA1C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11311,7 +11216,7 @@
         <xdr:cNvPr id="15" name="STOWAGE_PLAN_DEFAULT_SHAPE_542017">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F6C0C37-E6C7-4610-9B47-CF8A5D17D2D7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E055C08-F809-47EF-A2E1-E4743E886846}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11390,7 +11295,7 @@
         <xdr:cNvPr id="16" name="STOWAGE_PLAN_DEFAULT_SHAPE_428414">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62CD497E-A50A-47DA-BA5F-82E7729DCEBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA57C77E-EF9E-42C3-A550-B5D194EF23F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11456,7 +11361,7 @@
         <xdr:cNvPr id="17" name="Rectangle 710" descr="50%">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4C86EEE-FA2B-4C3A-AB86-9001A5274829}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6C6C50-5613-44C9-880E-7EC38603DA2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11535,88 +11440,69 @@
         </row>
         <row r="33">
           <cell r="J33">
-            <v>119</v>
+            <v>2</v>
           </cell>
           <cell r="AC33">
-            <v>121</v>
+            <v>2</v>
           </cell>
           <cell r="BG33">
-            <v>75</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="34">
           <cell r="J34">
-            <v>175.5</v>
+            <v>33.299999999999997</v>
           </cell>
           <cell r="AC34">
-            <v>195.6</v>
+            <v>15.5</v>
           </cell>
           <cell r="BG34">
-            <v>95.6</v>
+            <v>55.6</v>
           </cell>
         </row>
-        <row r="39">
-          <cell r="AC39">
+        <row r="40">
+          <cell r="BF40">
+            <v>22</v>
+          </cell>
+          <cell r="CA40">
             <v>2</v>
           </cell>
         </row>
-        <row r="40">
-          <cell r="P40">
-            <v>25</v>
-          </cell>
-          <cell r="AC40">
-            <v>152.30000000000001</v>
-          </cell>
-          <cell r="BF40">
-            <v>89</v>
-          </cell>
-          <cell r="CA40">
-            <v>55</v>
-          </cell>
-        </row>
         <row r="41">
-          <cell r="P41">
-            <v>135.30000000000001</v>
-          </cell>
           <cell r="BF41">
-            <v>12.3</v>
-          </cell>
-          <cell r="BP41">
-            <v>25</v>
+            <v>47.5</v>
           </cell>
           <cell r="CA41">
-            <v>12.3</v>
+            <v>15.6</v>
           </cell>
         </row>
         <row r="42">
           <cell r="H42">
             <v>34</v>
           </cell>
-          <cell r="BP42">
-            <v>50.3</v>
-          </cell>
         </row>
         <row r="43">
           <cell r="H43">
-            <v>135.30000000000001</v>
+            <v>15.6</v>
           </cell>
           <cell r="AE43">
-            <v>34</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="44">
           <cell r="AE44">
-            <v>152.30000000000001</v>
+            <v>78.8</v>
           </cell>
         </row>
-        <row r="49">
-          <cell r="CA49">
+        <row r="45">
+          <cell r="BD45">
             <v>55</v>
           </cell>
-        </row>
-        <row r="50">
-          <cell r="CA50">
-            <v>12.3</v>
+          <cell r="BG45">
+            <v>65.3</v>
+          </cell>
+          <cell r="BO45">
+            <v>25</v>
           </cell>
         </row>
         <row r="68">
@@ -11627,24 +11513,6 @@
         <row r="76">
           <cell r="AF76" t="str">
             <v xml:space="preserve"> </v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="AD106">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="AD107">
-            <v>135.30000000000001</v>
-          </cell>
-          <cell r="AV107">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="AV108">
-            <v>135.30000000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -11953,20 +11821,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA12F1F-CF42-4A02-ACE0-C83716FB98A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAE8C99C-B815-4C49-841F-2232B6FA48D7}">
   <sheetPr codeName="Sheet6">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:DF145"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="AT36" sqref="AT36"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="6" style="2" customWidth="1"/>
-    <col min="2" max="102" width="2.85546875" style="2" customWidth="1"/>
+    <col min="2" max="16" width="2.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="2" customWidth="1"/>
+    <col min="18" max="102" width="2.85546875" style="2" customWidth="1"/>
     <col min="103" max="103" width="2.85546875" style="3" customWidth="1"/>
     <col min="104" max="120" width="2.85546875" style="2" customWidth="1"/>
     <col min="121" max="16384" width="9.140625" style="2"/>
@@ -12673,84 +12541,84 @@
       <c r="AS9" s="47"/>
       <c r="AT9" s="48"/>
       <c r="AU9" s="49">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="AV9" s="50"/>
       <c r="AW9" s="50"/>
       <c r="AX9" s="50"/>
       <c r="AY9" s="50"/>
       <c r="AZ9" s="51">
-        <v>175.5</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="BA9" s="51"/>
       <c r="BB9" s="51"/>
       <c r="BC9" s="51"/>
       <c r="BD9" s="51"/>
       <c r="BE9" s="50">
-        <v>211</v>
+        <v>2</v>
       </c>
       <c r="BF9" s="50"/>
       <c r="BG9" s="50"/>
       <c r="BH9" s="50"/>
       <c r="BI9" s="50"/>
       <c r="BJ9" s="51">
-        <v>466.2</v>
+        <v>15.5</v>
       </c>
       <c r="BK9" s="51"/>
       <c r="BL9" s="51"/>
       <c r="BM9" s="51"/>
       <c r="BN9" s="51"/>
       <c r="BO9" s="50">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="BP9" s="50"/>
       <c r="BQ9" s="50"/>
       <c r="BR9" s="50"/>
       <c r="BS9" s="50"/>
       <c r="BT9" s="51">
-        <v>145.89999999999998</v>
+        <v>55.6</v>
       </c>
       <c r="BU9" s="51"/>
       <c r="BV9" s="51"/>
       <c r="BW9" s="51"/>
       <c r="BX9" s="51"/>
       <c r="BY9" s="50">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="BZ9" s="50"/>
       <c r="CA9" s="50"/>
       <c r="CB9" s="50"/>
       <c r="CC9" s="50"/>
       <c r="CD9" s="51">
-        <v>24.6</v>
+        <v>15.6</v>
       </c>
       <c r="CE9" s="51"/>
       <c r="CF9" s="51"/>
       <c r="CG9" s="51"/>
       <c r="CH9" s="52"/>
       <c r="CI9" s="53">
-        <v>540</v>
+        <v>8</v>
       </c>
       <c r="CJ9" s="54"/>
       <c r="CK9" s="54"/>
       <c r="CL9" s="54"/>
       <c r="CM9" s="55"/>
       <c r="CN9" s="56">
-        <v>812.2</v>
+        <v>120</v>
       </c>
       <c r="CO9" s="57"/>
       <c r="CP9" s="57"/>
       <c r="CQ9" s="57"/>
       <c r="CR9" s="58"/>
       <c r="CS9" s="49">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="CT9" s="50"/>
       <c r="CU9" s="50"/>
       <c r="CV9" s="50"/>
       <c r="CW9" s="50"/>
       <c r="CX9" s="51">
-        <v>482.5</v>
+        <v>12.5</v>
       </c>
       <c r="CY9" s="51"/>
       <c r="CZ9" s="51"/>
@@ -12820,28 +12688,28 @@
       <c r="BC10" s="69"/>
       <c r="BD10" s="69"/>
       <c r="BE10" s="68">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="BF10" s="68"/>
       <c r="BG10" s="68"/>
       <c r="BH10" s="68"/>
       <c r="BI10" s="68"/>
       <c r="BJ10" s="69">
-        <v>304.60000000000002</v>
+        <v>78.8</v>
       </c>
       <c r="BK10" s="69"/>
       <c r="BL10" s="69"/>
       <c r="BM10" s="69"/>
       <c r="BN10" s="69"/>
       <c r="BO10" s="68">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="BP10" s="68"/>
       <c r="BQ10" s="68"/>
       <c r="BR10" s="68"/>
       <c r="BS10" s="68"/>
       <c r="BT10" s="69">
-        <v>12.3</v>
+        <v>47.5</v>
       </c>
       <c r="BU10" s="69"/>
       <c r="BV10" s="69"/>
@@ -12858,14 +12726,14 @@
       <c r="CG10" s="69"/>
       <c r="CH10" s="70"/>
       <c r="CI10" s="71">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="CJ10" s="72"/>
       <c r="CK10" s="72"/>
       <c r="CL10" s="72"/>
       <c r="CM10" s="73"/>
       <c r="CN10" s="74">
-        <v>316.90000000000003</v>
+        <v>126.3</v>
       </c>
       <c r="CO10" s="75"/>
       <c r="CP10" s="75"/>
@@ -13165,14 +13033,14 @@
       <c r="AS13" s="65"/>
       <c r="AT13" s="66"/>
       <c r="AU13" s="67">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="AV13" s="68"/>
       <c r="AW13" s="68"/>
       <c r="AX13" s="68"/>
       <c r="AY13" s="68"/>
       <c r="AZ13" s="69">
-        <v>270.60000000000002</v>
+        <v>15.6</v>
       </c>
       <c r="BA13" s="69"/>
       <c r="BB13" s="69"/>
@@ -13188,12 +13056,16 @@
       <c r="BL13" s="69"/>
       <c r="BM13" s="69"/>
       <c r="BN13" s="69"/>
-      <c r="BO13" s="68"/>
+      <c r="BO13" s="68">
+        <v>55</v>
+      </c>
       <c r="BP13" s="68"/>
       <c r="BQ13" s="68"/>
       <c r="BR13" s="68"/>
       <c r="BS13" s="68"/>
-      <c r="BT13" s="69"/>
+      <c r="BT13" s="69">
+        <v>65.3</v>
+      </c>
       <c r="BU13" s="69"/>
       <c r="BV13" s="69"/>
       <c r="BW13" s="69"/>
@@ -13209,21 +13081,21 @@
       <c r="CG13" s="69"/>
       <c r="CH13" s="70"/>
       <c r="CI13" s="71">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="CJ13" s="72"/>
       <c r="CK13" s="72"/>
       <c r="CL13" s="72"/>
       <c r="CM13" s="73"/>
       <c r="CN13" s="74">
-        <v>270.60000000000002</v>
+        <v>80.899999999999991</v>
       </c>
       <c r="CO13" s="75"/>
       <c r="CP13" s="75"/>
       <c r="CQ13" s="75"/>
       <c r="CR13" s="76"/>
       <c r="CS13" s="67">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="CT13" s="68"/>
       <c r="CU13" s="68"/>
@@ -14481,56 +14353,56 @@
       <c r="AS25" s="33"/>
       <c r="AT25" s="34"/>
       <c r="AU25" s="122">
-        <v>178</v>
+        <v>36</v>
       </c>
       <c r="AV25" s="123"/>
       <c r="AW25" s="123"/>
       <c r="AX25" s="123"/>
       <c r="AY25" s="124"/>
       <c r="AZ25" s="122">
-        <v>446.1</v>
+        <v>48.9</v>
       </c>
       <c r="BA25" s="123"/>
       <c r="BB25" s="123"/>
       <c r="BC25" s="123"/>
       <c r="BD25" s="124"/>
       <c r="BE25" s="122">
-        <v>247</v>
+        <v>17</v>
       </c>
       <c r="BF25" s="123"/>
       <c r="BG25" s="123"/>
       <c r="BH25" s="123"/>
       <c r="BI25" s="124"/>
       <c r="BJ25" s="122">
-        <v>770.8</v>
+        <v>94.3</v>
       </c>
       <c r="BK25" s="123"/>
       <c r="BL25" s="123"/>
       <c r="BM25" s="123"/>
       <c r="BN25" s="124"/>
       <c r="BO25" s="122">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="BP25" s="123"/>
       <c r="BQ25" s="123"/>
       <c r="BR25" s="123"/>
       <c r="BS25" s="124"/>
       <c r="BT25" s="122">
-        <v>158.19999999999999</v>
+        <v>168.39999999999998</v>
       </c>
       <c r="BU25" s="123"/>
       <c r="BV25" s="123"/>
       <c r="BW25" s="123"/>
       <c r="BX25" s="124"/>
       <c r="BY25" s="122">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="BZ25" s="123"/>
       <c r="CA25" s="123"/>
       <c r="CB25" s="123"/>
       <c r="CC25" s="124"/>
       <c r="CD25" s="125">
-        <v>24.6</v>
+        <v>15.6</v>
       </c>
       <c r="CE25" s="126"/>
       <c r="CF25" s="126"/>
@@ -14619,28 +14491,28 @@
       <c r="CG26" s="129"/>
       <c r="CH26" s="133"/>
       <c r="CI26" s="130">
-        <v>724</v>
+        <v>159</v>
       </c>
       <c r="CJ26" s="131"/>
       <c r="CK26" s="131"/>
       <c r="CL26" s="131"/>
       <c r="CM26" s="132"/>
       <c r="CN26" s="134">
-        <v>1399.7000000000003</v>
+        <v>327.2</v>
       </c>
       <c r="CO26" s="135"/>
       <c r="CP26" s="135"/>
       <c r="CQ26" s="135"/>
       <c r="CR26" s="136"/>
       <c r="CS26" s="130">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="CT26" s="131"/>
       <c r="CU26" s="131"/>
       <c r="CV26" s="131"/>
       <c r="CW26" s="132"/>
       <c r="CX26" s="130">
-        <v>542.29999999999995</v>
+        <v>72.3</v>
       </c>
       <c r="CY26" s="131"/>
       <c r="CZ26" s="131"/>
@@ -15005,13 +14877,13 @@
       <c r="CJ31" s="149"/>
       <c r="CK31" s="149"/>
       <c r="CY31" s="150">
-        <v>315</v>
+        <v>6</v>
       </c>
       <c r="CZ31" s="151"/>
       <c r="DA31" s="151"/>
       <c r="DB31" s="152"/>
       <c r="DC31" s="1">
-        <v>315</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
@@ -15107,13 +14979,13 @@
       <c r="CJ32" s="149"/>
       <c r="CK32" s="149"/>
       <c r="CY32" s="158">
-        <v>466.70000000000005</v>
+        <v>104.4</v>
       </c>
       <c r="CZ32" s="159"/>
       <c r="DA32" s="159"/>
       <c r="DB32" s="160"/>
       <c r="DC32" s="1">
-        <v>466.70000000000005</v>
+        <v>104.4</v>
       </c>
     </row>
     <row r="33" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1">
@@ -15126,7 +14998,7 @@
       <c r="H33" s="142"/>
       <c r="I33" s="142"/>
       <c r="J33" s="161">
-        <v>119</v>
+        <v>2</v>
       </c>
       <c r="K33" s="162"/>
       <c r="L33" s="162"/>
@@ -15147,7 +15019,7 @@
       <c r="AA33" s="142"/>
       <c r="AB33" s="142"/>
       <c r="AC33" s="161">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="AD33" s="162"/>
       <c r="AE33" s="162"/>
@@ -15179,7 +15051,7 @@
       <c r="BE33" s="142"/>
       <c r="BF33" s="142"/>
       <c r="BG33" s="161">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="BH33" s="162"/>
       <c r="BI33" s="162"/>
@@ -15211,7 +15083,7 @@
       <c r="H34" s="142"/>
       <c r="I34" s="142"/>
       <c r="J34" s="167">
-        <v>175.5</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="K34" s="162"/>
       <c r="L34" s="162"/>
@@ -15232,7 +15104,7 @@
       <c r="AA34" s="142"/>
       <c r="AB34" s="142"/>
       <c r="AC34" s="167">
-        <v>195.6</v>
+        <v>15.5</v>
       </c>
       <c r="AD34" s="162"/>
       <c r="AE34" s="162"/>
@@ -15264,7 +15136,7 @@
       <c r="BE34" s="142"/>
       <c r="BF34" s="142"/>
       <c r="BG34" s="167">
-        <v>95.6</v>
+        <v>55.6</v>
       </c>
       <c r="BH34" s="162"/>
       <c r="BI34" s="162"/>
@@ -15649,14 +15521,12 @@
       <c r="Y39" s="180"/>
       <c r="Z39" s="181"/>
       <c r="AB39" s="180"/>
-      <c r="AC39" s="182">
-        <v>2</v>
-      </c>
-      <c r="AD39" s="183"/>
-      <c r="AE39" s="183"/>
+      <c r="AC39" s="182"/>
+      <c r="AD39" s="182"/>
+      <c r="AE39" s="182"/>
       <c r="AF39" s="180"/>
       <c r="AG39" s="180"/>
-      <c r="BB39" s="184"/>
+      <c r="BB39" s="183"/>
       <c r="BD39" s="180"/>
       <c r="BE39" s="180"/>
       <c r="BF39" s="180"/>
@@ -15666,8 +15536,8 @@
       <c r="BJ39" s="180"/>
       <c r="BK39" s="180"/>
       <c r="BY39" s="143"/>
-      <c r="CW39" s="184"/>
-      <c r="CY39" s="185" t="s">
+      <c r="CW39" s="183"/>
+      <c r="CY39" s="184" t="s">
         <v>34</v>
       </c>
     </row>
@@ -15686,12 +15556,10 @@
       <c r="M40" s="180"/>
       <c r="N40" s="180"/>
       <c r="O40" s="180"/>
-      <c r="P40" s="182">
-        <v>25</v>
-      </c>
-      <c r="Q40" s="183"/>
-      <c r="R40" s="183"/>
-      <c r="S40" s="183"/>
+      <c r="P40" s="182"/>
+      <c r="Q40" s="182"/>
+      <c r="R40" s="182"/>
+      <c r="S40" s="182"/>
       <c r="T40" s="180"/>
       <c r="U40" s="180"/>
       <c r="V40" s="180"/>
@@ -15700,40 +15568,38 @@
       <c r="Y40" s="180"/>
       <c r="Z40" s="181"/>
       <c r="AB40" s="180"/>
-      <c r="AC40" s="186">
-        <v>152.30000000000001</v>
-      </c>
-      <c r="AD40" s="183"/>
-      <c r="AE40" s="183"/>
+      <c r="AC40" s="182"/>
+      <c r="AD40" s="182"/>
+      <c r="AE40" s="182"/>
       <c r="AF40" s="180"/>
       <c r="AG40" s="180"/>
-      <c r="BB40" s="184"/>
+      <c r="BB40" s="183"/>
       <c r="BD40" s="180"/>
       <c r="BE40" s="180"/>
-      <c r="BF40" s="187">
-        <v>89</v>
-      </c>
-      <c r="BG40" s="188"/>
-      <c r="BH40" s="188"/>
-      <c r="BI40" s="188"/>
+      <c r="BF40" s="185">
+        <v>22</v>
+      </c>
+      <c r="BG40" s="186"/>
+      <c r="BH40" s="186"/>
+      <c r="BI40" s="186"/>
       <c r="BJ40" s="180"/>
-      <c r="BK40" s="189"/>
+      <c r="BK40" s="187"/>
       <c r="BY40" s="143"/>
-      <c r="CA40" s="190">
-        <v>55</v>
+      <c r="CA40" s="188">
+        <v>2</v>
       </c>
       <c r="CB40" s="168"/>
       <c r="CC40" s="168"/>
       <c r="CD40" s="168"/>
-      <c r="CW40" s="184"/>
+      <c r="CW40" s="183"/>
       <c r="CY40" s="150">
-        <v>264</v>
+        <v>153</v>
       </c>
       <c r="CZ40" s="151"/>
       <c r="DA40" s="151"/>
       <c r="DB40" s="152"/>
       <c r="DC40" s="1">
-        <v>264</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
@@ -15748,15 +15614,13 @@
       <c r="J41" s="180"/>
       <c r="K41" s="180"/>
       <c r="L41" s="180"/>
-      <c r="M41" s="189"/>
-      <c r="N41" s="189"/>
-      <c r="O41" s="189"/>
-      <c r="P41" s="186">
-        <v>135.30000000000001</v>
-      </c>
-      <c r="Q41" s="183"/>
-      <c r="R41" s="183"/>
-      <c r="S41" s="183"/>
+      <c r="M41" s="187"/>
+      <c r="N41" s="187"/>
+      <c r="O41" s="187"/>
+      <c r="P41" s="182"/>
+      <c r="Q41" s="182"/>
+      <c r="R41" s="182"/>
+      <c r="S41" s="182"/>
       <c r="T41" s="180"/>
       <c r="U41" s="180"/>
       <c r="V41" s="180"/>
@@ -15770,60 +15634,58 @@
       <c r="AE41" s="180"/>
       <c r="AF41" s="180"/>
       <c r="AG41" s="180"/>
-      <c r="AL41" s="191"/>
-      <c r="AM41" s="192"/>
-      <c r="AN41" s="192"/>
-      <c r="AO41" s="192"/>
-      <c r="AP41" s="192"/>
-      <c r="AQ41" s="192"/>
-      <c r="AR41" s="192"/>
-      <c r="AS41" s="192"/>
-      <c r="AT41" s="192"/>
-      <c r="AU41" s="192"/>
-      <c r="AV41" s="193"/>
-      <c r="BB41" s="184"/>
+      <c r="AL41" s="189"/>
+      <c r="AM41" s="190"/>
+      <c r="AN41" s="190"/>
+      <c r="AO41" s="190"/>
+      <c r="AP41" s="190"/>
+      <c r="AQ41" s="190"/>
+      <c r="AR41" s="190"/>
+      <c r="AS41" s="190"/>
+      <c r="AT41" s="190"/>
+      <c r="AU41" s="190"/>
+      <c r="AV41" s="191"/>
+      <c r="BB41" s="183"/>
       <c r="BD41" s="180"/>
       <c r="BE41" s="180"/>
-      <c r="BF41" s="194">
-        <v>12.3</v>
-      </c>
-      <c r="BG41" s="188"/>
-      <c r="BH41" s="188"/>
-      <c r="BI41" s="188"/>
+      <c r="BF41" s="192">
+        <v>47.5</v>
+      </c>
+      <c r="BG41" s="186"/>
+      <c r="BH41" s="186"/>
+      <c r="BI41" s="186"/>
       <c r="BJ41" s="180"/>
       <c r="BK41" s="180"/>
-      <c r="BP41" s="190">
-        <v>25</v>
-      </c>
+      <c r="BP41" s="168"/>
       <c r="BQ41" s="168"/>
       <c r="BR41" s="168"/>
       <c r="BS41" s="168"/>
       <c r="BY41" s="143"/>
-      <c r="CA41" s="195">
-        <v>12.3</v>
+      <c r="CA41" s="193">
+        <v>15.6</v>
       </c>
       <c r="CB41" s="168"/>
       <c r="CC41" s="168"/>
       <c r="CD41" s="168"/>
-      <c r="CH41" s="191"/>
-      <c r="CI41" s="192"/>
-      <c r="CJ41" s="192"/>
-      <c r="CK41" s="192"/>
-      <c r="CL41" s="192"/>
-      <c r="CM41" s="192"/>
-      <c r="CN41" s="192"/>
-      <c r="CO41" s="192"/>
-      <c r="CP41" s="192"/>
-      <c r="CQ41" s="193"/>
-      <c r="CW41" s="184"/>
+      <c r="CH41" s="189"/>
+      <c r="CI41" s="190"/>
+      <c r="CJ41" s="190"/>
+      <c r="CK41" s="190"/>
+      <c r="CL41" s="190"/>
+      <c r="CM41" s="190"/>
+      <c r="CN41" s="190"/>
+      <c r="CO41" s="190"/>
+      <c r="CP41" s="190"/>
+      <c r="CQ41" s="191"/>
+      <c r="CW41" s="183"/>
       <c r="CY41" s="158">
-        <v>650.10000000000014</v>
+        <v>222.8</v>
       </c>
       <c r="CZ41" s="159"/>
       <c r="DA41" s="159"/>
       <c r="DB41" s="160"/>
       <c r="DC41" s="1">
-        <v>650.10000000000014</v>
+        <v>222.8</v>
       </c>
     </row>
     <row r="42" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1">
@@ -15833,15 +15695,15 @@
       <c r="E42" s="180"/>
       <c r="F42" s="180"/>
       <c r="G42" s="180"/>
-      <c r="H42" s="182">
+      <c r="H42" s="194">
         <v>34</v>
       </c>
-      <c r="I42" s="183"/>
-      <c r="J42" s="183"/>
-      <c r="K42" s="183"/>
+      <c r="I42" s="182"/>
+      <c r="J42" s="182"/>
+      <c r="K42" s="182"/>
       <c r="L42" s="180"/>
       <c r="M42" s="180"/>
-      <c r="N42" s="189"/>
+      <c r="N42" s="187"/>
       <c r="O42" s="180"/>
       <c r="P42" s="180"/>
       <c r="Q42" s="180"/>
@@ -15860,18 +15722,18 @@
       <c r="AE42" s="180"/>
       <c r="AF42" s="180"/>
       <c r="AG42" s="180"/>
-      <c r="AL42" s="196"/>
-      <c r="AM42" s="197"/>
-      <c r="AN42" s="197"/>
-      <c r="AO42" s="197"/>
-      <c r="AP42" s="197"/>
-      <c r="AQ42" s="197"/>
-      <c r="AR42" s="197"/>
-      <c r="AS42" s="197"/>
-      <c r="AT42" s="197"/>
-      <c r="AU42" s="197"/>
-      <c r="AV42" s="198"/>
-      <c r="BB42" s="184"/>
+      <c r="AL42" s="195"/>
+      <c r="AM42" s="196"/>
+      <c r="AN42" s="196"/>
+      <c r="AO42" s="196"/>
+      <c r="AP42" s="196"/>
+      <c r="AQ42" s="196"/>
+      <c r="AR42" s="196"/>
+      <c r="AS42" s="196"/>
+      <c r="AT42" s="196"/>
+      <c r="AU42" s="196"/>
+      <c r="AV42" s="197"/>
+      <c r="BB42" s="183"/>
       <c r="BD42" s="180"/>
       <c r="BE42" s="180"/>
       <c r="BF42" s="180"/>
@@ -15880,24 +15742,22 @@
       <c r="BI42" s="180"/>
       <c r="BJ42" s="180"/>
       <c r="BK42" s="180"/>
-      <c r="BP42" s="195">
-        <v>50.3</v>
-      </c>
+      <c r="BP42" s="168"/>
       <c r="BQ42" s="168"/>
       <c r="BR42" s="168"/>
       <c r="BS42" s="168"/>
       <c r="BY42" s="143"/>
-      <c r="CH42" s="196"/>
-      <c r="CI42" s="197"/>
-      <c r="CJ42" s="197"/>
-      <c r="CK42" s="197"/>
-      <c r="CL42" s="197"/>
-      <c r="CM42" s="197"/>
-      <c r="CN42" s="197"/>
-      <c r="CO42" s="197"/>
-      <c r="CP42" s="197"/>
-      <c r="CQ42" s="198"/>
-      <c r="CW42" s="184"/>
+      <c r="CH42" s="195"/>
+      <c r="CI42" s="196"/>
+      <c r="CJ42" s="196"/>
+      <c r="CK42" s="196"/>
+      <c r="CL42" s="196"/>
+      <c r="CM42" s="196"/>
+      <c r="CN42" s="196"/>
+      <c r="CO42" s="196"/>
+      <c r="CP42" s="196"/>
+      <c r="CQ42" s="197"/>
+      <c r="CW42" s="183"/>
       <c r="CY42" s="166" t="s">
         <v>36</v>
       </c>
@@ -15912,12 +15772,12 @@
       <c r="E43" s="180"/>
       <c r="F43" s="180"/>
       <c r="G43" s="180"/>
-      <c r="H43" s="186">
-        <v>135.30000000000001</v>
-      </c>
-      <c r="I43" s="183"/>
-      <c r="J43" s="183"/>
-      <c r="K43" s="183"/>
+      <c r="H43" s="198">
+        <v>15.6</v>
+      </c>
+      <c r="I43" s="182"/>
+      <c r="J43" s="182"/>
+      <c r="K43" s="182"/>
       <c r="L43" s="180"/>
       <c r="M43" s="180"/>
       <c r="N43" s="180"/>
@@ -15936,12 +15796,12 @@
       <c r="AB43" s="180"/>
       <c r="AC43" s="180"/>
       <c r="AD43" s="180"/>
-      <c r="AE43" s="182">
-        <v>34</v>
-      </c>
-      <c r="AF43" s="183"/>
-      <c r="AG43" s="183"/>
-      <c r="BB43" s="184"/>
+      <c r="AE43" s="194">
+        <v>15</v>
+      </c>
+      <c r="AF43" s="182"/>
+      <c r="AG43" s="182"/>
+      <c r="BB43" s="183"/>
       <c r="BD43" s="180"/>
       <c r="BE43" s="180"/>
       <c r="BF43" s="180"/>
@@ -15951,7 +15811,7 @@
       <c r="BJ43" s="180"/>
       <c r="BK43" s="180"/>
       <c r="BY43" s="143"/>
-      <c r="CW43" s="184"/>
+      <c r="CW43" s="183"/>
       <c r="CY43" s="169" t="s">
         <v>67</v>
       </c>
@@ -15982,20 +15842,20 @@
       <c r="U44" s="180"/>
       <c r="V44" s="180"/>
       <c r="W44" s="180"/>
-      <c r="X44" s="189"/>
+      <c r="X44" s="187"/>
       <c r="Y44" s="180"/>
       <c r="Z44" s="181"/>
       <c r="AB44" s="180"/>
       <c r="AC44" s="180"/>
       <c r="AD44" s="180"/>
-      <c r="AE44" s="186">
-        <v>152.30000000000001</v>
-      </c>
-      <c r="AF44" s="183"/>
-      <c r="AG44" s="183"/>
-      <c r="BB44" s="184"/>
+      <c r="AE44" s="198">
+        <v>78.8</v>
+      </c>
+      <c r="AF44" s="182"/>
+      <c r="AG44" s="182"/>
+      <c r="BB44" s="183"/>
       <c r="BY44" s="143"/>
-      <c r="CW44" s="184"/>
+      <c r="CW44" s="183"/>
     </row>
     <row r="45" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B45" s="179"/>
@@ -16017,10 +15877,10 @@
       <c r="R45" s="180"/>
       <c r="S45" s="180"/>
       <c r="T45" s="180"/>
-      <c r="U45" s="189"/>
-      <c r="V45" s="189"/>
-      <c r="W45" s="189"/>
-      <c r="X45" s="189"/>
+      <c r="U45" s="187"/>
+      <c r="V45" s="187"/>
+      <c r="W45" s="187"/>
+      <c r="X45" s="187"/>
       <c r="Y45" s="180"/>
       <c r="Z45" s="181"/>
       <c r="AB45" s="180"/>
@@ -16028,12 +15888,27 @@
       <c r="AD45" s="180"/>
       <c r="AE45" s="180"/>
       <c r="AF45" s="180"/>
-      <c r="AG45" s="189"/>
+      <c r="AG45" s="187"/>
       <c r="AH45" s="12"/>
       <c r="AI45" s="12"/>
-      <c r="BB45" s="184"/>
+      <c r="BB45" s="183"/>
+      <c r="BD45" s="194">
+        <v>55</v>
+      </c>
+      <c r="BE45" s="182"/>
+      <c r="BF45" s="182"/>
+      <c r="BG45" s="198">
+        <v>65.3</v>
+      </c>
+      <c r="BH45" s="182"/>
+      <c r="BI45" s="182"/>
+      <c r="BO45" s="194">
+        <v>25</v>
+      </c>
+      <c r="BP45" s="182"/>
+      <c r="BQ45" s="182"/>
       <c r="BY45" s="143"/>
-      <c r="CW45" s="184"/>
+      <c r="CW45" s="183"/>
     </row>
     <row r="46" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B46" s="179"/>
@@ -16067,9 +15942,10 @@
       <c r="AE46" s="180"/>
       <c r="AF46" s="180"/>
       <c r="AG46" s="180"/>
-      <c r="BB46" s="184"/>
+      <c r="BB46" s="183"/>
+      <c r="BO46" s="180"/>
       <c r="BY46" s="143"/>
-      <c r="CW46" s="184"/>
+      <c r="CW46" s="183"/>
     </row>
     <row r="47" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B47" s="177"/>
@@ -16178,57 +16054,53 @@
     </row>
     <row r="48" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B48" s="143"/>
-      <c r="Z48" s="184"/>
-      <c r="BB48" s="184"/>
+      <c r="Z48" s="183"/>
+      <c r="BB48" s="183"/>
       <c r="BY48" s="143"/>
-      <c r="CW48" s="184"/>
+      <c r="CW48" s="183"/>
       <c r="CY48" s="199" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="49" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B49" s="143"/>
-      <c r="Z49" s="184"/>
-      <c r="BB49" s="184"/>
+      <c r="Z49" s="183"/>
+      <c r="BB49" s="183"/>
       <c r="BY49" s="143"/>
-      <c r="CA49" s="190">
-        <v>55</v>
-      </c>
+      <c r="CA49" s="168"/>
       <c r="CB49" s="168"/>
       <c r="CC49" s="168"/>
       <c r="CD49" s="168"/>
-      <c r="CW49" s="184"/>
+      <c r="CW49" s="183"/>
       <c r="CY49" s="150">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="CZ49" s="151"/>
       <c r="DA49" s="151"/>
       <c r="DB49" s="152"/>
       <c r="DC49" s="1">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B50" s="143"/>
-      <c r="Z50" s="184"/>
-      <c r="AL50" s="191"/>
-      <c r="AM50" s="192"/>
-      <c r="AN50" s="192"/>
-      <c r="AO50" s="192"/>
-      <c r="AP50" s="192"/>
-      <c r="AQ50" s="192"/>
-      <c r="AR50" s="192"/>
-      <c r="AS50" s="192"/>
-      <c r="AT50" s="192"/>
-      <c r="AU50" s="192"/>
-      <c r="AV50" s="193"/>
-      <c r="BB50" s="184"/>
+      <c r="Z50" s="183"/>
+      <c r="AL50" s="189"/>
+      <c r="AM50" s="190"/>
+      <c r="AN50" s="190"/>
+      <c r="AO50" s="190"/>
+      <c r="AP50" s="190"/>
+      <c r="AQ50" s="190"/>
+      <c r="AR50" s="190"/>
+      <c r="AS50" s="190"/>
+      <c r="AT50" s="190"/>
+      <c r="AU50" s="190"/>
+      <c r="AV50" s="191"/>
+      <c r="BB50" s="183"/>
       <c r="BL50" s="12"/>
       <c r="BM50" s="12"/>
       <c r="BY50" s="143"/>
-      <c r="CA50" s="195">
-        <v>12.3</v>
-      </c>
+      <c r="CA50" s="168"/>
       <c r="CB50" s="168"/>
       <c r="CC50" s="168"/>
       <c r="CD50" s="168"/>
@@ -16244,32 +16116,32 @@
       <c r="CP50" s="201"/>
       <c r="CQ50" s="201"/>
       <c r="CR50" s="202"/>
-      <c r="CW50" s="184"/>
+      <c r="CW50" s="183"/>
       <c r="CY50" s="158">
-        <v>12.3</v>
+        <v>0</v>
       </c>
       <c r="CZ50" s="159"/>
       <c r="DA50" s="159"/>
       <c r="DB50" s="160"/>
       <c r="DC50" s="1">
-        <v>12.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="B51" s="143"/>
-      <c r="Z51" s="184"/>
-      <c r="AL51" s="196"/>
-      <c r="AM51" s="197"/>
-      <c r="AN51" s="197"/>
-      <c r="AO51" s="197"/>
-      <c r="AP51" s="197"/>
-      <c r="AQ51" s="197"/>
-      <c r="AR51" s="197"/>
-      <c r="AS51" s="197"/>
-      <c r="AT51" s="197"/>
-      <c r="AU51" s="197"/>
-      <c r="AV51" s="198"/>
-      <c r="BB51" s="184"/>
+      <c r="Z51" s="183"/>
+      <c r="AL51" s="195"/>
+      <c r="AM51" s="196"/>
+      <c r="AN51" s="196"/>
+      <c r="AO51" s="196"/>
+      <c r="AP51" s="196"/>
+      <c r="AQ51" s="196"/>
+      <c r="AR51" s="196"/>
+      <c r="AS51" s="196"/>
+      <c r="AT51" s="196"/>
+      <c r="AU51" s="196"/>
+      <c r="AV51" s="197"/>
+      <c r="BB51" s="183"/>
       <c r="BL51" s="12"/>
       <c r="BY51" s="143"/>
       <c r="CG51" s="203"/>
@@ -16284,43 +16156,43 @@
       <c r="CP51" s="204"/>
       <c r="CQ51" s="204"/>
       <c r="CR51" s="205"/>
-      <c r="CW51" s="184"/>
+      <c r="CW51" s="183"/>
       <c r="CY51" s="206" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="52" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B52" s="143"/>
-      <c r="Z52" s="184"/>
-      <c r="BB52" s="184"/>
+      <c r="Z52" s="183"/>
+      <c r="BB52" s="183"/>
       <c r="BY52" s="143"/>
-      <c r="CW52" s="184"/>
+      <c r="CW52" s="183"/>
       <c r="CY52" s="207" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B53" s="143"/>
-      <c r="Z53" s="184"/>
-      <c r="BB53" s="184"/>
+      <c r="Z53" s="183"/>
+      <c r="BB53" s="183"/>
       <c r="BY53" s="143"/>
-      <c r="CW53" s="184"/>
+      <c r="CW53" s="183"/>
       <c r="CY53" s="206"/>
     </row>
     <row r="54" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B54" s="143"/>
-      <c r="Z54" s="184"/>
-      <c r="BB54" s="184"/>
+      <c r="Z54" s="183"/>
+      <c r="BB54" s="183"/>
       <c r="BY54" s="143"/>
-      <c r="CW54" s="184"/>
+      <c r="CW54" s="183"/>
       <c r="CY54" s="207"/>
     </row>
     <row r="55" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B55" s="143"/>
-      <c r="Z55" s="184"/>
-      <c r="BB55" s="184"/>
+      <c r="Z55" s="183"/>
+      <c r="BB55" s="183"/>
       <c r="BY55" s="143"/>
-      <c r="CW55" s="184"/>
+      <c r="CW55" s="183"/>
     </row>
     <row r="56" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B56" s="177"/>
@@ -16429,20 +16301,20 @@
     </row>
     <row r="57" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B57" s="143"/>
-      <c r="Z57" s="184"/>
-      <c r="BB57" s="184"/>
-      <c r="BX57" s="184"/>
-      <c r="CW57" s="184"/>
-      <c r="CY57" s="185" t="s">
+      <c r="Z57" s="183"/>
+      <c r="BB57" s="183"/>
+      <c r="BX57" s="183"/>
+      <c r="CW57" s="183"/>
+      <c r="CY57" s="184" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="58" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B58" s="143"/>
-      <c r="Z58" s="184"/>
-      <c r="BB58" s="184"/>
-      <c r="BX58" s="184"/>
-      <c r="CW58" s="184"/>
+      <c r="Z58" s="183"/>
+      <c r="BB58" s="183"/>
+      <c r="BX58" s="183"/>
+      <c r="CW58" s="183"/>
       <c r="CY58" s="150">
         <v>0</v>
       </c>
@@ -16455,7 +16327,7 @@
     </row>
     <row r="59" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B59" s="143"/>
-      <c r="Z59" s="184"/>
+      <c r="Z59" s="183"/>
       <c r="AL59" s="200"/>
       <c r="AM59" s="201"/>
       <c r="AN59" s="201"/>
@@ -16467,22 +16339,22 @@
       <c r="AT59" s="201"/>
       <c r="AU59" s="201"/>
       <c r="AV59" s="202"/>
-      <c r="BB59" s="184"/>
-      <c r="BX59" s="184"/>
-      <c r="BY59" s="192"/>
-      <c r="BZ59" s="192"/>
-      <c r="CA59" s="192"/>
-      <c r="CB59" s="192"/>
-      <c r="CC59" s="192"/>
-      <c r="CD59" s="192"/>
-      <c r="CE59" s="192"/>
-      <c r="CF59" s="192"/>
-      <c r="CG59" s="192"/>
-      <c r="CH59" s="192"/>
-      <c r="CI59" s="192"/>
-      <c r="CJ59" s="192"/>
-      <c r="CK59" s="193"/>
-      <c r="CW59" s="184"/>
+      <c r="BB59" s="183"/>
+      <c r="BX59" s="183"/>
+      <c r="BY59" s="190"/>
+      <c r="BZ59" s="190"/>
+      <c r="CA59" s="190"/>
+      <c r="CB59" s="190"/>
+      <c r="CC59" s="190"/>
+      <c r="CD59" s="190"/>
+      <c r="CE59" s="190"/>
+      <c r="CF59" s="190"/>
+      <c r="CG59" s="190"/>
+      <c r="CH59" s="190"/>
+      <c r="CI59" s="190"/>
+      <c r="CJ59" s="190"/>
+      <c r="CK59" s="191"/>
+      <c r="CW59" s="183"/>
       <c r="CY59" s="158">
         <v>0</v>
       </c>
@@ -16495,7 +16367,7 @@
     </row>
     <row r="60" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="B60" s="143"/>
-      <c r="Z60" s="184"/>
+      <c r="Z60" s="183"/>
       <c r="AL60" s="203"/>
       <c r="AM60" s="204"/>
       <c r="AN60" s="204"/>
@@ -16507,56 +16379,56 @@
       <c r="AT60" s="204"/>
       <c r="AU60" s="204"/>
       <c r="AV60" s="205"/>
-      <c r="BB60" s="184"/>
-      <c r="BX60" s="184"/>
-      <c r="BY60" s="197"/>
-      <c r="BZ60" s="197"/>
-      <c r="CA60" s="197"/>
-      <c r="CB60" s="197"/>
-      <c r="CC60" s="197"/>
-      <c r="CD60" s="197"/>
-      <c r="CE60" s="197"/>
-      <c r="CF60" s="197"/>
-      <c r="CG60" s="197"/>
-      <c r="CH60" s="197"/>
-      <c r="CI60" s="197"/>
-      <c r="CJ60" s="197"/>
-      <c r="CK60" s="198"/>
-      <c r="CW60" s="184"/>
+      <c r="BB60" s="183"/>
+      <c r="BX60" s="183"/>
+      <c r="BY60" s="196"/>
+      <c r="BZ60" s="196"/>
+      <c r="CA60" s="196"/>
+      <c r="CB60" s="196"/>
+      <c r="CC60" s="196"/>
+      <c r="CD60" s="196"/>
+      <c r="CE60" s="196"/>
+      <c r="CF60" s="196"/>
+      <c r="CG60" s="196"/>
+      <c r="CH60" s="196"/>
+      <c r="CI60" s="196"/>
+      <c r="CJ60" s="196"/>
+      <c r="CK60" s="197"/>
+      <c r="CW60" s="183"/>
       <c r="CY60" s="206" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B61" s="143"/>
-      <c r="Z61" s="184"/>
-      <c r="BB61" s="184"/>
-      <c r="BX61" s="184"/>
-      <c r="CW61" s="184"/>
+      <c r="Z61" s="183"/>
+      <c r="BB61" s="183"/>
+      <c r="BX61" s="183"/>
+      <c r="CW61" s="183"/>
       <c r="CY61" s="207" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="62" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B62" s="143"/>
-      <c r="Z62" s="184"/>
-      <c r="BB62" s="184"/>
-      <c r="BX62" s="184"/>
-      <c r="CW62" s="184"/>
+      <c r="Z62" s="183"/>
+      <c r="BB62" s="183"/>
+      <c r="BX62" s="183"/>
+      <c r="CW62" s="183"/>
     </row>
     <row r="63" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B63" s="143"/>
-      <c r="Z63" s="184"/>
-      <c r="BB63" s="184"/>
+      <c r="Z63" s="183"/>
+      <c r="BB63" s="183"/>
       <c r="BY63" s="143"/>
-      <c r="CW63" s="184"/>
+      <c r="CW63" s="183"/>
     </row>
     <row r="64" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B64" s="143"/>
-      <c r="Z64" s="184"/>
-      <c r="BB64" s="184"/>
+      <c r="Z64" s="183"/>
+      <c r="BB64" s="183"/>
       <c r="BY64" s="143"/>
-      <c r="CW64" s="184"/>
+      <c r="CW64" s="183"/>
     </row>
     <row r="65" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B65" s="177"/>
@@ -16673,27 +16545,27 @@
     </row>
     <row r="66" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B66" s="143"/>
-      <c r="Z66" s="184"/>
-      <c r="BB66" s="184"/>
-      <c r="BX66" s="184"/>
-      <c r="CW66" s="184"/>
+      <c r="Z66" s="183"/>
+      <c r="BB66" s="183"/>
+      <c r="BX66" s="183"/>
+      <c r="CW66" s="183"/>
       <c r="CY66" s="212" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="67" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B67" s="143"/>
-      <c r="Z67" s="184"/>
-      <c r="BB67" s="184"/>
-      <c r="BX67" s="184"/>
-      <c r="CW67" s="184"/>
+      <c r="Z67" s="183"/>
+      <c r="BB67" s="183"/>
+      <c r="BX67" s="183"/>
+      <c r="CW67" s="183"/>
       <c r="CY67" s="213" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="68" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B68" s="143"/>
-      <c r="Z68" s="184"/>
+      <c r="Z68" s="183"/>
       <c r="AF68" s="214" t="s">
         <v>32</v>
       </c>
@@ -16713,20 +16585,20 @@
       <c r="AT68" s="217"/>
       <c r="AU68" s="217"/>
       <c r="AV68" s="218"/>
-      <c r="BB68" s="184"/>
-      <c r="BH68" s="191"/>
-      <c r="BI68" s="192"/>
-      <c r="BJ68" s="192"/>
-      <c r="BK68" s="192"/>
-      <c r="BL68" s="192"/>
-      <c r="BM68" s="192"/>
-      <c r="BN68" s="192"/>
-      <c r="BO68" s="192"/>
-      <c r="BP68" s="192"/>
-      <c r="BQ68" s="192"/>
-      <c r="BR68" s="192"/>
-      <c r="BS68" s="193"/>
-      <c r="BX68" s="184"/>
+      <c r="BB68" s="183"/>
+      <c r="BH68" s="189"/>
+      <c r="BI68" s="190"/>
+      <c r="BJ68" s="190"/>
+      <c r="BK68" s="190"/>
+      <c r="BL68" s="190"/>
+      <c r="BM68" s="190"/>
+      <c r="BN68" s="190"/>
+      <c r="BO68" s="190"/>
+      <c r="BP68" s="190"/>
+      <c r="BQ68" s="190"/>
+      <c r="BR68" s="190"/>
+      <c r="BS68" s="191"/>
+      <c r="BX68" s="183"/>
       <c r="BY68" s="219"/>
       <c r="BZ68" s="201"/>
       <c r="CA68" s="201"/>
@@ -16739,14 +16611,14 @@
       <c r="CH68" s="201"/>
       <c r="CI68" s="201"/>
       <c r="CJ68" s="202"/>
-      <c r="CW68" s="184"/>
+      <c r="CW68" s="183"/>
       <c r="CY68" s="213" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="69" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B69" s="143"/>
-      <c r="Z69" s="184"/>
+      <c r="Z69" s="183"/>
       <c r="AF69" s="220"/>
       <c r="AG69" s="221"/>
       <c r="AH69" s="221"/>
@@ -16764,20 +16636,20 @@
       <c r="AT69" s="224"/>
       <c r="AU69" s="224"/>
       <c r="AV69" s="225"/>
-      <c r="BB69" s="184"/>
-      <c r="BH69" s="196"/>
-      <c r="BI69" s="197"/>
-      <c r="BJ69" s="197"/>
-      <c r="BK69" s="197"/>
-      <c r="BL69" s="197"/>
-      <c r="BM69" s="197"/>
-      <c r="BN69" s="197"/>
-      <c r="BO69" s="197"/>
-      <c r="BP69" s="197"/>
-      <c r="BQ69" s="197"/>
-      <c r="BR69" s="197"/>
-      <c r="BS69" s="198"/>
-      <c r="BX69" s="184"/>
+      <c r="BB69" s="183"/>
+      <c r="BH69" s="195"/>
+      <c r="BI69" s="196"/>
+      <c r="BJ69" s="196"/>
+      <c r="BK69" s="196"/>
+      <c r="BL69" s="196"/>
+      <c r="BM69" s="196"/>
+      <c r="BN69" s="196"/>
+      <c r="BO69" s="196"/>
+      <c r="BP69" s="196"/>
+      <c r="BQ69" s="196"/>
+      <c r="BR69" s="196"/>
+      <c r="BS69" s="197"/>
+      <c r="BX69" s="183"/>
       <c r="BY69" s="226"/>
       <c r="BZ69" s="204"/>
       <c r="CA69" s="204"/>
@@ -16790,7 +16662,7 @@
       <c r="CH69" s="204"/>
       <c r="CI69" s="204"/>
       <c r="CJ69" s="205"/>
-      <c r="CW69" s="184"/>
+      <c r="CW69" s="183"/>
       <c r="CY69" s="150">
         <v>0</v>
       </c>
@@ -16803,10 +16675,10 @@
     </row>
     <row r="70" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B70" s="143"/>
-      <c r="Z70" s="184"/>
-      <c r="BB70" s="184"/>
-      <c r="BX70" s="184"/>
-      <c r="CW70" s="184"/>
+      <c r="Z70" s="183"/>
+      <c r="BB70" s="183"/>
+      <c r="BX70" s="183"/>
+      <c r="CW70" s="183"/>
       <c r="CY70" s="158">
         <v>0</v>
       </c>
@@ -16819,30 +16691,30 @@
     </row>
     <row r="71" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="B71" s="143"/>
-      <c r="Z71" s="184"/>
-      <c r="BB71" s="184"/>
-      <c r="BX71" s="184"/>
-      <c r="CW71" s="184"/>
+      <c r="Z71" s="183"/>
+      <c r="BB71" s="183"/>
+      <c r="BX71" s="183"/>
+      <c r="CW71" s="183"/>
       <c r="CY71" s="227" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="72" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B72" s="143"/>
-      <c r="Z72" s="184"/>
-      <c r="BB72" s="184"/>
-      <c r="BX72" s="184"/>
-      <c r="CW72" s="184"/>
+      <c r="Z72" s="183"/>
+      <c r="BB72" s="183"/>
+      <c r="BX72" s="183"/>
+      <c r="CW72" s="183"/>
       <c r="CY72" s="206" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="73" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B73" s="143"/>
-      <c r="Z73" s="184"/>
-      <c r="BB73" s="184"/>
+      <c r="Z73" s="183"/>
+      <c r="BB73" s="183"/>
       <c r="BX73" s="228"/>
-      <c r="CW73" s="184"/>
+      <c r="CW73" s="183"/>
     </row>
     <row r="74" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B74" s="175"/>
@@ -16950,9 +16822,9 @@
       </c>
     </row>
     <row r="75" spans="2:109" ht="20.100000000000001" customHeight="1">
-      <c r="F75" s="184"/>
-      <c r="Z75" s="184"/>
-      <c r="BB75" s="184"/>
+      <c r="F75" s="183"/>
+      <c r="Z75" s="183"/>
+      <c r="BB75" s="183"/>
       <c r="BY75" s="143"/>
       <c r="CO75" s="143"/>
       <c r="CY75" s="213" t="s">
@@ -16960,8 +16832,8 @@
       </c>
     </row>
     <row r="76" spans="2:109" ht="20.100000000000001" customHeight="1">
-      <c r="F76" s="184"/>
-      <c r="Z76" s="184"/>
+      <c r="F76" s="183"/>
+      <c r="Z76" s="183"/>
       <c r="AF76" s="200" t="s">
         <v>32</v>
       </c>
@@ -16981,7 +16853,7 @@
       <c r="AT76" s="217"/>
       <c r="AU76" s="217"/>
       <c r="AV76" s="218"/>
-      <c r="BB76" s="184"/>
+      <c r="BB76" s="183"/>
       <c r="BE76" s="12"/>
       <c r="BF76" s="12"/>
       <c r="BG76" s="12"/>
@@ -16992,8 +16864,8 @@
       </c>
     </row>
     <row r="77" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="F77" s="184"/>
-      <c r="Z77" s="184"/>
+      <c r="F77" s="183"/>
+      <c r="Z77" s="183"/>
       <c r="AF77" s="203"/>
       <c r="AG77" s="204"/>
       <c r="AH77" s="204"/>
@@ -17003,15 +16875,15 @@
       <c r="AL77" s="204"/>
       <c r="AM77" s="204"/>
       <c r="AN77" s="205"/>
-      <c r="AO77" s="197"/>
-      <c r="AP77" s="197"/>
-      <c r="AQ77" s="197"/>
-      <c r="AR77" s="197"/>
-      <c r="AS77" s="197"/>
-      <c r="AT77" s="197"/>
-      <c r="AU77" s="197"/>
-      <c r="AV77" s="198"/>
-      <c r="BB77" s="184"/>
+      <c r="AO77" s="196"/>
+      <c r="AP77" s="196"/>
+      <c r="AQ77" s="196"/>
+      <c r="AR77" s="196"/>
+      <c r="AS77" s="196"/>
+      <c r="AT77" s="196"/>
+      <c r="AU77" s="196"/>
+      <c r="AV77" s="197"/>
+      <c r="BB77" s="183"/>
       <c r="BE77" s="12"/>
       <c r="BF77" s="12"/>
       <c r="BG77" s="12"/>
@@ -17041,9 +16913,9 @@
       </c>
     </row>
     <row r="78" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="F78" s="184"/>
-      <c r="Z78" s="184"/>
-      <c r="BB78" s="184"/>
+      <c r="F78" s="183"/>
+      <c r="Z78" s="183"/>
+      <c r="BB78" s="183"/>
       <c r="BH78" s="203"/>
       <c r="BI78" s="204"/>
       <c r="BJ78" s="204"/>
@@ -17076,9 +16948,9 @@
       </c>
     </row>
     <row r="79" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
-      <c r="F79" s="184"/>
-      <c r="Z79" s="184"/>
-      <c r="BB79" s="184"/>
+      <c r="F79" s="183"/>
+      <c r="Z79" s="183"/>
+      <c r="BB79" s="183"/>
       <c r="BY79" s="231"/>
       <c r="CO79" s="143"/>
       <c r="CY79" s="158">
@@ -17092,9 +16964,9 @@
       </c>
     </row>
     <row r="80" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="F80" s="184"/>
-      <c r="Z80" s="184"/>
-      <c r="BB80" s="184"/>
+      <c r="F80" s="183"/>
+      <c r="Z80" s="183"/>
+      <c r="BB80" s="183"/>
       <c r="BY80" s="143"/>
       <c r="CO80" s="143"/>
       <c r="CY80" s="206" t="s">
@@ -17102,9 +16974,9 @@
       </c>
     </row>
     <row r="81" spans="2:109" ht="20.100000000000001" customHeight="1">
-      <c r="F81" s="184"/>
-      <c r="Z81" s="184"/>
-      <c r="BB81" s="184"/>
+      <c r="F81" s="183"/>
+      <c r="Z81" s="183"/>
+      <c r="BB81" s="183"/>
       <c r="BY81" s="143"/>
       <c r="CO81" s="143"/>
       <c r="CY81" s="207" t="s">
@@ -17112,9 +16984,9 @@
       </c>
     </row>
     <row r="82" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="F82" s="184"/>
-      <c r="Z82" s="184"/>
-      <c r="BB82" s="184"/>
+      <c r="F82" s="183"/>
+      <c r="Z82" s="183"/>
+      <c r="BB82" s="183"/>
       <c r="BY82" s="143"/>
       <c r="CO82" s="143"/>
     </row>
@@ -17227,8 +17099,8 @@
     </row>
     <row r="84" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B84" s="143"/>
-      <c r="Z84" s="184"/>
-      <c r="BB84" s="184"/>
+      <c r="Z84" s="183"/>
+      <c r="BB84" s="183"/>
       <c r="BY84" s="143"/>
       <c r="CQ84" s="143"/>
       <c r="CY84" s="213" t="s">
@@ -17237,8 +17109,8 @@
     </row>
     <row r="85" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B85" s="143"/>
-      <c r="Z85" s="184"/>
-      <c r="BB85" s="184"/>
+      <c r="Z85" s="183"/>
+      <c r="BB85" s="183"/>
       <c r="BY85" s="143"/>
       <c r="CQ85" s="143"/>
       <c r="CY85" s="212" t="s">
@@ -17247,19 +17119,19 @@
     </row>
     <row r="86" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B86" s="143"/>
-      <c r="Z86" s="184"/>
-      <c r="AC86" s="191"/>
-      <c r="AD86" s="192"/>
-      <c r="AE86" s="192"/>
-      <c r="AF86" s="192"/>
-      <c r="AG86" s="192"/>
-      <c r="AH86" s="192"/>
-      <c r="AI86" s="192"/>
-      <c r="AJ86" s="192"/>
-      <c r="AK86" s="192"/>
-      <c r="AL86" s="192"/>
-      <c r="AM86" s="192"/>
-      <c r="AN86" s="193"/>
+      <c r="Z86" s="183"/>
+      <c r="AC86" s="189"/>
+      <c r="AD86" s="190"/>
+      <c r="AE86" s="190"/>
+      <c r="AF86" s="190"/>
+      <c r="AG86" s="190"/>
+      <c r="AH86" s="190"/>
+      <c r="AI86" s="190"/>
+      <c r="AJ86" s="190"/>
+      <c r="AK86" s="190"/>
+      <c r="AL86" s="190"/>
+      <c r="AM86" s="190"/>
+      <c r="AN86" s="191"/>
       <c r="AO86" s="236"/>
       <c r="AP86" s="224"/>
       <c r="AQ86" s="224"/>
@@ -17268,27 +17140,27 @@
       <c r="AT86" s="224"/>
       <c r="AU86" s="224"/>
       <c r="AV86" s="225"/>
-      <c r="BB86" s="184"/>
-      <c r="BH86" s="191"/>
-      <c r="BI86" s="192"/>
-      <c r="BJ86" s="192"/>
-      <c r="BK86" s="192"/>
-      <c r="BL86" s="192"/>
-      <c r="BM86" s="192"/>
-      <c r="BN86" s="192"/>
-      <c r="BO86" s="192"/>
-      <c r="BP86" s="192"/>
-      <c r="BQ86" s="192"/>
-      <c r="BR86" s="192"/>
-      <c r="BS86" s="193"/>
-      <c r="BT86" s="191"/>
-      <c r="BU86" s="192"/>
-      <c r="BV86" s="192"/>
-      <c r="BW86" s="192"/>
-      <c r="BX86" s="192"/>
+      <c r="BB86" s="183"/>
+      <c r="BH86" s="189"/>
+      <c r="BI86" s="190"/>
+      <c r="BJ86" s="190"/>
+      <c r="BK86" s="190"/>
+      <c r="BL86" s="190"/>
+      <c r="BM86" s="190"/>
+      <c r="BN86" s="190"/>
+      <c r="BO86" s="190"/>
+      <c r="BP86" s="190"/>
+      <c r="BQ86" s="190"/>
+      <c r="BR86" s="190"/>
+      <c r="BS86" s="191"/>
+      <c r="BT86" s="189"/>
+      <c r="BU86" s="190"/>
+      <c r="BV86" s="190"/>
+      <c r="BW86" s="190"/>
+      <c r="BX86" s="190"/>
       <c r="BY86" s="231"/>
-      <c r="BZ86" s="192"/>
-      <c r="CA86" s="193"/>
+      <c r="BZ86" s="190"/>
+      <c r="CA86" s="191"/>
       <c r="CQ86" s="143"/>
       <c r="CY86" s="213" t="s">
         <v>39</v>
@@ -17296,19 +17168,19 @@
     </row>
     <row r="87" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B87" s="143"/>
-      <c r="Z87" s="184"/>
-      <c r="AC87" s="196"/>
-      <c r="AD87" s="197"/>
-      <c r="AE87" s="197"/>
-      <c r="AF87" s="197"/>
-      <c r="AG87" s="197"/>
-      <c r="AH87" s="197"/>
-      <c r="AI87" s="197"/>
-      <c r="AJ87" s="197"/>
-      <c r="AK87" s="197"/>
-      <c r="AL87" s="197"/>
-      <c r="AM87" s="197"/>
-      <c r="AN87" s="198"/>
+      <c r="Z87" s="183"/>
+      <c r="AC87" s="195"/>
+      <c r="AD87" s="196"/>
+      <c r="AE87" s="196"/>
+      <c r="AF87" s="196"/>
+      <c r="AG87" s="196"/>
+      <c r="AH87" s="196"/>
+      <c r="AI87" s="196"/>
+      <c r="AJ87" s="196"/>
+      <c r="AK87" s="196"/>
+      <c r="AL87" s="196"/>
+      <c r="AM87" s="196"/>
+      <c r="AN87" s="197"/>
       <c r="AO87" s="237"/>
       <c r="AP87" s="217"/>
       <c r="AQ87" s="217"/>
@@ -17317,27 +17189,27 @@
       <c r="AT87" s="217"/>
       <c r="AU87" s="217"/>
       <c r="AV87" s="218"/>
-      <c r="BB87" s="184"/>
-      <c r="BH87" s="196"/>
-      <c r="BI87" s="197"/>
-      <c r="BJ87" s="197"/>
-      <c r="BK87" s="197"/>
-      <c r="BL87" s="197"/>
-      <c r="BM87" s="197"/>
-      <c r="BN87" s="197"/>
-      <c r="BO87" s="197"/>
-      <c r="BP87" s="197"/>
-      <c r="BQ87" s="197"/>
-      <c r="BR87" s="197"/>
-      <c r="BS87" s="198"/>
-      <c r="BT87" s="196"/>
-      <c r="BU87" s="197"/>
-      <c r="BV87" s="197"/>
-      <c r="BW87" s="197"/>
-      <c r="BX87" s="197"/>
+      <c r="BB87" s="183"/>
+      <c r="BH87" s="195"/>
+      <c r="BI87" s="196"/>
+      <c r="BJ87" s="196"/>
+      <c r="BK87" s="196"/>
+      <c r="BL87" s="196"/>
+      <c r="BM87" s="196"/>
+      <c r="BN87" s="196"/>
+      <c r="BO87" s="196"/>
+      <c r="BP87" s="196"/>
+      <c r="BQ87" s="196"/>
+      <c r="BR87" s="196"/>
+      <c r="BS87" s="197"/>
+      <c r="BT87" s="195"/>
+      <c r="BU87" s="196"/>
+      <c r="BV87" s="196"/>
+      <c r="BW87" s="196"/>
+      <c r="BX87" s="196"/>
       <c r="BY87" s="230"/>
-      <c r="BZ87" s="197"/>
-      <c r="CA87" s="198"/>
+      <c r="BZ87" s="196"/>
+      <c r="CA87" s="197"/>
       <c r="CQ87" s="143"/>
       <c r="CY87" s="150">
         <v>0</v>
@@ -17351,8 +17223,8 @@
     </row>
     <row r="88" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B88" s="143"/>
-      <c r="Z88" s="184"/>
-      <c r="BB88" s="184"/>
+      <c r="Z88" s="183"/>
+      <c r="BB88" s="183"/>
       <c r="BY88" s="143"/>
       <c r="CQ88" s="143"/>
       <c r="CY88" s="158">
@@ -17367,8 +17239,8 @@
     </row>
     <row r="89" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="B89" s="143"/>
-      <c r="Z89" s="184"/>
-      <c r="BB89" s="184"/>
+      <c r="Z89" s="183"/>
+      <c r="BB89" s="183"/>
       <c r="BY89" s="143"/>
       <c r="CQ89" s="143"/>
       <c r="CY89" s="206" t="s">
@@ -17377,8 +17249,8 @@
     </row>
     <row r="90" spans="2:109" ht="20.100000000000001" customHeight="1">
       <c r="B90" s="143"/>
-      <c r="Z90" s="184"/>
-      <c r="BB90" s="184"/>
+      <c r="Z90" s="183"/>
+      <c r="BB90" s="183"/>
       <c r="BY90" s="143"/>
       <c r="CQ90" s="143"/>
       <c r="CY90" s="207" t="s">
@@ -17387,8 +17259,8 @@
     </row>
     <row r="91" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B91" s="143"/>
-      <c r="Z91" s="184"/>
-      <c r="BB91" s="184"/>
+      <c r="Z91" s="183"/>
+      <c r="BB91" s="183"/>
       <c r="BY91" s="143"/>
       <c r="CQ91" s="143"/>
     </row>
@@ -17507,8 +17379,8 @@
       <c r="N93" s="204"/>
       <c r="O93" s="204"/>
       <c r="P93" s="205"/>
-      <c r="Z93" s="184"/>
-      <c r="BB93" s="184"/>
+      <c r="Z93" s="183"/>
+      <c r="BB93" s="183"/>
       <c r="BY93" s="143"/>
       <c r="CQ93" s="143"/>
       <c r="CY93" s="213" t="s">
@@ -17517,8 +17389,8 @@
     </row>
     <row r="94" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B94" s="143"/>
-      <c r="Z94" s="184"/>
-      <c r="BB94" s="184"/>
+      <c r="Z94" s="183"/>
+      <c r="BB94" s="183"/>
       <c r="BY94" s="143"/>
       <c r="CQ94" s="143"/>
       <c r="CY94" s="212" t="s">
@@ -17527,7 +17399,7 @@
     </row>
     <row r="95" spans="2:109" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B95" s="143"/>
-      <c r="Z95" s="184"/>
+      <c r="Z95" s="183"/>
       <c r="AC95" s="200"/>
       <c r="AD95" s="201"/>
       <c r="AE95" s="201"/>
@@ -17550,7 +17422,7 @@
       <c r="AV95" s="243"/>
       <c r="AW95" s="243"/>
       <c r="AX95" s="244"/>
-      <c r="BB95" s="184"/>
+      <c r="BB95" s="183"/>
       <c r="BH95" s="200"/>
       <c r="BI95" s="201"/>
       <c r="BJ95" s="201"/>
@@ -17566,7 +17438,7 @@
     </row>
     <row r="96" spans="2:109" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B96" s="143"/>
-      <c r="Z96" s="184"/>
+      <c r="Z96" s="183"/>
       <c r="AC96" s="245"/>
       <c r="AD96" s="246"/>
       <c r="AE96" s="246"/>
@@ -17580,7 +17452,7 @@
       <c r="AM96" s="12"/>
       <c r="AN96" s="12"/>
       <c r="AX96" s="248"/>
-      <c r="BB96" s="184"/>
+      <c r="BB96" s="183"/>
       <c r="BH96" s="245"/>
       <c r="BI96" s="246"/>
       <c r="BJ96" s="246"/>
@@ -17602,7 +17474,7 @@
     </row>
     <row r="97" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="B97" s="143"/>
-      <c r="Z97" s="184"/>
+      <c r="Z97" s="183"/>
       <c r="AC97" s="203"/>
       <c r="AD97" s="204"/>
       <c r="AE97" s="204"/>
@@ -17625,7 +17497,7 @@
       <c r="AV97" s="250"/>
       <c r="AW97" s="250"/>
       <c r="AX97" s="251"/>
-      <c r="BB97" s="184"/>
+      <c r="BB97" s="183"/>
       <c r="BH97" s="203"/>
       <c r="BI97" s="204"/>
       <c r="BJ97" s="204"/>
@@ -17647,10 +17519,10 @@
     </row>
     <row r="98" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B98" s="143"/>
-      <c r="Z98" s="184"/>
+      <c r="Z98" s="183"/>
       <c r="AH98" s="252"/>
       <c r="AR98" s="253"/>
-      <c r="BB98" s="184"/>
+      <c r="BB98" s="183"/>
       <c r="BI98" s="254"/>
       <c r="BJ98" s="255"/>
       <c r="BK98" s="255"/>
@@ -17670,10 +17542,10 @@
     </row>
     <row r="99" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B99" s="143"/>
-      <c r="Z99" s="184"/>
+      <c r="Z99" s="183"/>
       <c r="AH99" s="252"/>
       <c r="AR99" s="253"/>
-      <c r="BB99" s="184"/>
+      <c r="BB99" s="183"/>
       <c r="BI99" s="252"/>
       <c r="BS99" s="253"/>
       <c r="BY99" s="143"/>
@@ -17684,7 +17556,7 @@
     </row>
     <row r="100" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B100" s="143"/>
-      <c r="Z100" s="184"/>
+      <c r="Z100" s="183"/>
       <c r="AH100" s="257"/>
       <c r="AI100" s="258"/>
       <c r="AJ100" s="258"/>
@@ -17696,7 +17568,7 @@
       <c r="AP100" s="258"/>
       <c r="AQ100" s="258"/>
       <c r="AR100" s="259"/>
-      <c r="BB100" s="184"/>
+      <c r="BB100" s="183"/>
       <c r="BI100" s="257"/>
       <c r="BJ100" s="258"/>
       <c r="BK100" s="258"/>
@@ -17709,24 +17581,24 @@
       <c r="BR100" s="258"/>
       <c r="BS100" s="259"/>
       <c r="BY100" s="143"/>
-      <c r="CP100" s="184"/>
+      <c r="CP100" s="183"/>
       <c r="CQ100" s="143"/>
     </row>
     <row r="101" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B101" s="143"/>
-      <c r="Z101" s="184"/>
-      <c r="BB101" s="184"/>
+      <c r="Z101" s="183"/>
+      <c r="BB101" s="183"/>
       <c r="BY101" s="143"/>
-      <c r="CP101" s="184"/>
+      <c r="CP101" s="183"/>
       <c r="CQ101" s="143"/>
     </row>
     <row r="102" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="B102" s="143"/>
       <c r="Y102" s="200"/>
       <c r="Z102" s="260"/>
-      <c r="BB102" s="184"/>
+      <c r="BB102" s="183"/>
       <c r="BY102" s="143"/>
-      <c r="CP102" s="184"/>
+      <c r="CP102" s="183"/>
       <c r="CQ102" s="143"/>
     </row>
     <row r="103" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -17764,9 +17636,9 @@
       <c r="AG103" s="264"/>
       <c r="AH103" s="264"/>
       <c r="AI103" s="265"/>
-      <c r="BB103" s="184"/>
+      <c r="BB103" s="183"/>
       <c r="BY103" s="143"/>
-      <c r="CP103" s="184"/>
+      <c r="CP103" s="183"/>
       <c r="CQ103" s="143"/>
     </row>
     <row r="104" spans="2:107" ht="20.100000000000001" customHeight="1">
@@ -17844,59 +17716,53 @@
     </row>
     <row r="105" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA105" s="143"/>
-      <c r="BB105" s="184"/>
+      <c r="BB105" s="183"/>
       <c r="BY105" s="143"/>
-      <c r="CP105" s="184"/>
-      <c r="CY105" s="185" t="s">
+      <c r="CP105" s="183"/>
+      <c r="CY105" s="184" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="106" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA106" s="143"/>
-      <c r="AD106" s="190">
-        <v>45</v>
-      </c>
+      <c r="AD106" s="168"/>
       <c r="AE106" s="168"/>
       <c r="AF106" s="168"/>
       <c r="AG106" s="168"/>
-      <c r="BB106" s="184"/>
+      <c r="BB106" s="183"/>
       <c r="BY106" s="143"/>
-      <c r="CP106" s="184"/>
+      <c r="CP106" s="183"/>
       <c r="CY106" s="150">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="CZ106" s="151"/>
       <c r="DA106" s="151"/>
       <c r="DB106" s="152"/>
       <c r="DC106" s="1">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA107" s="143"/>
-      <c r="AD107" s="195">
-        <v>135.30000000000001</v>
-      </c>
+      <c r="AD107" s="168"/>
       <c r="AE107" s="168"/>
       <c r="AF107" s="168"/>
       <c r="AG107" s="168"/>
-      <c r="AV107" s="190">
-        <v>45</v>
-      </c>
+      <c r="AV107" s="168"/>
       <c r="AW107" s="168"/>
       <c r="AX107" s="168"/>
       <c r="AY107" s="168"/>
-      <c r="BB107" s="184"/>
+      <c r="BB107" s="183"/>
       <c r="BY107" s="143"/>
-      <c r="CP107" s="184"/>
+      <c r="CP107" s="183"/>
       <c r="CY107" s="158">
-        <v>270.60000000000002</v>
+        <v>0</v>
       </c>
       <c r="CZ107" s="159"/>
       <c r="DA107" s="159"/>
       <c r="DB107" s="160"/>
       <c r="DC107" s="1">
-        <v>270.60000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:107" ht="20.100000000000001" customHeight="1" thickTop="1">
@@ -17912,13 +17778,11 @@
       <c r="AP108" s="201"/>
       <c r="AQ108" s="201"/>
       <c r="AR108" s="202"/>
-      <c r="AV108" s="195">
-        <v>135.30000000000001</v>
-      </c>
+      <c r="AV108" s="168"/>
       <c r="AW108" s="168"/>
       <c r="AX108" s="168"/>
       <c r="AY108" s="168"/>
-      <c r="BB108" s="184"/>
+      <c r="BB108" s="183"/>
       <c r="BI108" s="200"/>
       <c r="BJ108" s="201"/>
       <c r="BK108" s="201"/>
@@ -17931,7 +17795,7 @@
       <c r="BR108" s="201"/>
       <c r="BS108" s="202"/>
       <c r="BY108" s="143"/>
-      <c r="CP108" s="184"/>
+      <c r="CP108" s="183"/>
       <c r="CY108" s="206" t="s">
         <v>40</v>
       </c>
@@ -17949,7 +17813,7 @@
       <c r="AP109" s="204"/>
       <c r="AQ109" s="204"/>
       <c r="AR109" s="205"/>
-      <c r="BB109" s="184"/>
+      <c r="BB109" s="183"/>
       <c r="BI109" s="203"/>
       <c r="BJ109" s="204"/>
       <c r="BK109" s="204"/>
@@ -17962,28 +17826,28 @@
       <c r="BR109" s="204"/>
       <c r="BS109" s="205"/>
       <c r="BY109" s="143"/>
-      <c r="CP109" s="184"/>
+      <c r="CP109" s="183"/>
       <c r="CY109" s="207" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="110" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="AA110" s="143"/>
-      <c r="BB110" s="184"/>
+      <c r="BB110" s="183"/>
       <c r="BY110" s="143"/>
-      <c r="CP110" s="184"/>
+      <c r="CP110" s="183"/>
     </row>
     <row r="111" spans="2:107" ht="20.100000000000001" customHeight="1">
       <c r="AA111" s="143"/>
-      <c r="BB111" s="184"/>
+      <c r="BB111" s="183"/>
       <c r="BY111" s="143"/>
-      <c r="CP111" s="184"/>
+      <c r="CP111" s="183"/>
     </row>
     <row r="112" spans="2:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA112" s="143"/>
-      <c r="BB112" s="184"/>
+      <c r="BB112" s="183"/>
       <c r="BY112" s="143"/>
-      <c r="CP112" s="184"/>
+      <c r="CP112" s="183"/>
     </row>
     <row r="113" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA113" s="177"/>
@@ -18061,19 +17925,19 @@
     </row>
     <row r="114" spans="27:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA114" s="143"/>
-      <c r="BB114" s="184"/>
+      <c r="BB114" s="183"/>
       <c r="BY114" s="143"/>
-      <c r="CK114" s="184"/>
+      <c r="CK114" s="183"/>
       <c r="CX114" s="269"/>
-      <c r="CY114" s="185" t="s">
+      <c r="CY114" s="184" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="115" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA115" s="143"/>
-      <c r="BB115" s="184"/>
+      <c r="BB115" s="183"/>
       <c r="BY115" s="143"/>
-      <c r="CK115" s="184"/>
+      <c r="CK115" s="183"/>
       <c r="CX115" s="269"/>
       <c r="CY115" s="150">
         <v>0</v>
@@ -18087,9 +17951,9 @@
     </row>
     <row r="116" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA116" s="143"/>
-      <c r="BB116" s="184"/>
+      <c r="BB116" s="183"/>
       <c r="BY116" s="143"/>
-      <c r="CK116" s="184"/>
+      <c r="CK116" s="183"/>
       <c r="CY116" s="158">
         <v>0</v>
       </c>
@@ -18102,81 +17966,81 @@
     </row>
     <row r="117" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="AA117" s="143"/>
-      <c r="AH117" s="191"/>
-      <c r="AI117" s="192"/>
-      <c r="AJ117" s="192"/>
-      <c r="AK117" s="192"/>
-      <c r="AL117" s="192"/>
-      <c r="AM117" s="192"/>
-      <c r="AN117" s="192"/>
-      <c r="AO117" s="192"/>
-      <c r="AP117" s="192"/>
-      <c r="AQ117" s="192"/>
-      <c r="AR117" s="193"/>
-      <c r="BB117" s="184"/>
-      <c r="BI117" s="191"/>
-      <c r="BJ117" s="192"/>
-      <c r="BK117" s="192"/>
-      <c r="BL117" s="192"/>
-      <c r="BM117" s="192"/>
-      <c r="BN117" s="192"/>
-      <c r="BO117" s="192"/>
-      <c r="BP117" s="192"/>
-      <c r="BQ117" s="192"/>
-      <c r="BR117" s="192"/>
-      <c r="BS117" s="193"/>
+      <c r="AH117" s="189"/>
+      <c r="AI117" s="190"/>
+      <c r="AJ117" s="190"/>
+      <c r="AK117" s="190"/>
+      <c r="AL117" s="190"/>
+      <c r="AM117" s="190"/>
+      <c r="AN117" s="190"/>
+      <c r="AO117" s="190"/>
+      <c r="AP117" s="190"/>
+      <c r="AQ117" s="190"/>
+      <c r="AR117" s="191"/>
+      <c r="BB117" s="183"/>
+      <c r="BI117" s="189"/>
+      <c r="BJ117" s="190"/>
+      <c r="BK117" s="190"/>
+      <c r="BL117" s="190"/>
+      <c r="BM117" s="190"/>
+      <c r="BN117" s="190"/>
+      <c r="BO117" s="190"/>
+      <c r="BP117" s="190"/>
+      <c r="BQ117" s="190"/>
+      <c r="BR117" s="190"/>
+      <c r="BS117" s="191"/>
       <c r="BY117" s="143"/>
-      <c r="CK117" s="184"/>
+      <c r="CK117" s="183"/>
       <c r="CY117" s="206" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="118" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA118" s="143"/>
-      <c r="AH118" s="196"/>
-      <c r="AI118" s="197"/>
-      <c r="AJ118" s="197"/>
-      <c r="AK118" s="197"/>
-      <c r="AL118" s="197"/>
-      <c r="AM118" s="197"/>
-      <c r="AN118" s="197"/>
-      <c r="AO118" s="197"/>
-      <c r="AP118" s="197"/>
-      <c r="AQ118" s="197"/>
-      <c r="AR118" s="198"/>
-      <c r="BB118" s="184"/>
-      <c r="BI118" s="196"/>
-      <c r="BJ118" s="197"/>
-      <c r="BK118" s="197"/>
-      <c r="BL118" s="197"/>
-      <c r="BM118" s="197"/>
-      <c r="BN118" s="197"/>
-      <c r="BO118" s="197"/>
-      <c r="BP118" s="197"/>
-      <c r="BQ118" s="197"/>
-      <c r="BR118" s="197"/>
-      <c r="BS118" s="198"/>
+      <c r="AH118" s="195"/>
+      <c r="AI118" s="196"/>
+      <c r="AJ118" s="196"/>
+      <c r="AK118" s="196"/>
+      <c r="AL118" s="196"/>
+      <c r="AM118" s="196"/>
+      <c r="AN118" s="196"/>
+      <c r="AO118" s="196"/>
+      <c r="AP118" s="196"/>
+      <c r="AQ118" s="196"/>
+      <c r="AR118" s="197"/>
+      <c r="BB118" s="183"/>
+      <c r="BI118" s="195"/>
+      <c r="BJ118" s="196"/>
+      <c r="BK118" s="196"/>
+      <c r="BL118" s="196"/>
+      <c r="BM118" s="196"/>
+      <c r="BN118" s="196"/>
+      <c r="BO118" s="196"/>
+      <c r="BP118" s="196"/>
+      <c r="BQ118" s="196"/>
+      <c r="BR118" s="196"/>
+      <c r="BS118" s="197"/>
       <c r="BY118" s="143"/>
-      <c r="CK118" s="184"/>
+      <c r="CK118" s="183"/>
       <c r="CY118" s="207" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="119" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA119" s="143"/>
-      <c r="BB119" s="184"/>
+      <c r="BB119" s="183"/>
       <c r="BY119" s="143"/>
-      <c r="CK119" s="184"/>
+      <c r="CK119" s="183"/>
     </row>
     <row r="120" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA120" s="143"/>
-      <c r="BB120" s="184"/>
+      <c r="BB120" s="183"/>
       <c r="BY120" s="143"/>
-      <c r="CK120" s="184"/>
+      <c r="CK120" s="183"/>
     </row>
     <row r="121" spans="27:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA121" s="143"/>
-      <c r="BB121" s="184"/>
+      <c r="BB121" s="183"/>
       <c r="BY121" s="261"/>
       <c r="BZ121" s="262"/>
       <c r="CA121" s="262"/>
@@ -18248,19 +18112,19 @@
     </row>
     <row r="123" spans="27:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA123" s="143"/>
-      <c r="BB123" s="184"/>
-      <c r="BX123" s="184"/>
+      <c r="BB123" s="183"/>
+      <c r="BX123" s="183"/>
       <c r="CA123" s="270" t="s">
         <v>59</v>
       </c>
-      <c r="CY123" s="185" t="s">
+      <c r="CY123" s="184" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="124" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA124" s="143"/>
-      <c r="BB124" s="184"/>
-      <c r="BX124" s="184"/>
+      <c r="BB124" s="183"/>
+      <c r="BX124" s="183"/>
       <c r="CA124" s="10" t="s">
         <v>60</v>
       </c>
@@ -18276,8 +18140,8 @@
     </row>
     <row r="125" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA125" s="143"/>
-      <c r="BB125" s="184"/>
-      <c r="BX125" s="184"/>
+      <c r="BB125" s="183"/>
+      <c r="BX125" s="183"/>
       <c r="CY125" s="158">
         <v>0</v>
       </c>
@@ -18290,78 +18154,78 @@
     </row>
     <row r="126" spans="27:107" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="AA126" s="143"/>
-      <c r="AH126" s="191"/>
-      <c r="AI126" s="192"/>
-      <c r="AJ126" s="192"/>
-      <c r="AK126" s="192"/>
-      <c r="AL126" s="192"/>
-      <c r="AM126" s="192"/>
-      <c r="AN126" s="192"/>
-      <c r="AO126" s="192"/>
-      <c r="AP126" s="192"/>
-      <c r="AQ126" s="192"/>
-      <c r="AR126" s="193"/>
-      <c r="BB126" s="184"/>
-      <c r="BI126" s="191"/>
-      <c r="BJ126" s="192"/>
-      <c r="BK126" s="192"/>
-      <c r="BL126" s="192"/>
-      <c r="BM126" s="192"/>
-      <c r="BN126" s="192"/>
-      <c r="BO126" s="192"/>
-      <c r="BP126" s="192"/>
-      <c r="BQ126" s="192"/>
-      <c r="BR126" s="192"/>
-      <c r="BS126" s="193"/>
-      <c r="BX126" s="184"/>
+      <c r="AH126" s="189"/>
+      <c r="AI126" s="190"/>
+      <c r="AJ126" s="190"/>
+      <c r="AK126" s="190"/>
+      <c r="AL126" s="190"/>
+      <c r="AM126" s="190"/>
+      <c r="AN126" s="190"/>
+      <c r="AO126" s="190"/>
+      <c r="AP126" s="190"/>
+      <c r="AQ126" s="190"/>
+      <c r="AR126" s="191"/>
+      <c r="BB126" s="183"/>
+      <c r="BI126" s="189"/>
+      <c r="BJ126" s="190"/>
+      <c r="BK126" s="190"/>
+      <c r="BL126" s="190"/>
+      <c r="BM126" s="190"/>
+      <c r="BN126" s="190"/>
+      <c r="BO126" s="190"/>
+      <c r="BP126" s="190"/>
+      <c r="BQ126" s="190"/>
+      <c r="BR126" s="190"/>
+      <c r="BS126" s="191"/>
+      <c r="BX126" s="183"/>
       <c r="CY126" s="206" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="127" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA127" s="143"/>
-      <c r="AH127" s="196"/>
-      <c r="AI127" s="197"/>
-      <c r="AJ127" s="197"/>
-      <c r="AK127" s="197"/>
-      <c r="AL127" s="197"/>
-      <c r="AM127" s="197"/>
-      <c r="AN127" s="197"/>
-      <c r="AO127" s="197"/>
-      <c r="AP127" s="197"/>
-      <c r="AQ127" s="197"/>
-      <c r="AR127" s="198"/>
-      <c r="BB127" s="184"/>
-      <c r="BI127" s="196"/>
-      <c r="BJ127" s="197"/>
-      <c r="BK127" s="197"/>
-      <c r="BL127" s="197"/>
-      <c r="BM127" s="197"/>
-      <c r="BN127" s="197"/>
-      <c r="BO127" s="197"/>
-      <c r="BP127" s="197"/>
-      <c r="BQ127" s="197"/>
-      <c r="BR127" s="197"/>
-      <c r="BS127" s="198"/>
-      <c r="BX127" s="184"/>
+      <c r="AH127" s="195"/>
+      <c r="AI127" s="196"/>
+      <c r="AJ127" s="196"/>
+      <c r="AK127" s="196"/>
+      <c r="AL127" s="196"/>
+      <c r="AM127" s="196"/>
+      <c r="AN127" s="196"/>
+      <c r="AO127" s="196"/>
+      <c r="AP127" s="196"/>
+      <c r="AQ127" s="196"/>
+      <c r="AR127" s="197"/>
+      <c r="BB127" s="183"/>
+      <c r="BI127" s="195"/>
+      <c r="BJ127" s="196"/>
+      <c r="BK127" s="196"/>
+      <c r="BL127" s="196"/>
+      <c r="BM127" s="196"/>
+      <c r="BN127" s="196"/>
+      <c r="BO127" s="196"/>
+      <c r="BP127" s="196"/>
+      <c r="BQ127" s="196"/>
+      <c r="BR127" s="196"/>
+      <c r="BS127" s="197"/>
+      <c r="BX127" s="183"/>
       <c r="CY127" s="207" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="128" spans="27:107" ht="20.100000000000001" customHeight="1">
       <c r="AA128" s="143"/>
-      <c r="BB128" s="184"/>
-      <c r="BX128" s="184"/>
+      <c r="BB128" s="183"/>
+      <c r="BX128" s="183"/>
     </row>
     <row r="129" spans="5:107" ht="20.100000000000001" customHeight="1">
       <c r="AA129" s="143"/>
-      <c r="BB129" s="184"/>
-      <c r="BX129" s="184"/>
+      <c r="BB129" s="183"/>
+      <c r="BX129" s="183"/>
     </row>
     <row r="130" spans="5:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA130" s="143"/>
-      <c r="BB130" s="184"/>
-      <c r="BX130" s="184"/>
+      <c r="BB130" s="183"/>
+      <c r="BX130" s="183"/>
     </row>
     <row r="131" spans="5:107" ht="20.100000000000001" customHeight="1">
       <c r="AA131" s="177"/>
@@ -18420,16 +18284,16 @@
     </row>
     <row r="132" spans="5:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA132" s="143"/>
-      <c r="BB132" s="184"/>
-      <c r="BX132" s="184"/>
-      <c r="CY132" s="185" t="s">
+      <c r="BB132" s="183"/>
+      <c r="BX132" s="183"/>
+      <c r="CY132" s="184" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="133" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA133" s="143"/>
-      <c r="BB133" s="184"/>
-      <c r="BX133" s="184"/>
+      <c r="BB133" s="183"/>
+      <c r="BX133" s="183"/>
       <c r="CY133" s="150">
         <v>0</v>
       </c>
@@ -18442,8 +18306,8 @@
     </row>
     <row r="134" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA134" s="143"/>
-      <c r="BB134" s="184"/>
-      <c r="BX134" s="184"/>
+      <c r="BB134" s="183"/>
+      <c r="BX134" s="183"/>
       <c r="CY134" s="158">
         <v>0</v>
       </c>
@@ -18456,73 +18320,73 @@
     </row>
     <row r="135" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1">
       <c r="AA135" s="143"/>
-      <c r="AH135" s="191"/>
-      <c r="AI135" s="192"/>
-      <c r="AJ135" s="192"/>
-      <c r="AK135" s="192"/>
-      <c r="AL135" s="192"/>
-      <c r="AM135" s="192"/>
-      <c r="AN135" s="192"/>
-      <c r="AO135" s="192"/>
-      <c r="AP135" s="192"/>
-      <c r="AQ135" s="192"/>
-      <c r="AR135" s="193"/>
-      <c r="BB135" s="184"/>
-      <c r="BI135" s="191"/>
-      <c r="BJ135" s="192"/>
-      <c r="BK135" s="192"/>
-      <c r="BL135" s="192"/>
-      <c r="BM135" s="192"/>
-      <c r="BN135" s="192"/>
-      <c r="BO135" s="192"/>
-      <c r="BP135" s="192"/>
-      <c r="BQ135" s="192"/>
-      <c r="BR135" s="192"/>
-      <c r="BS135" s="193"/>
-      <c r="BX135" s="184"/>
+      <c r="AH135" s="189"/>
+      <c r="AI135" s="190"/>
+      <c r="AJ135" s="190"/>
+      <c r="AK135" s="190"/>
+      <c r="AL135" s="190"/>
+      <c r="AM135" s="190"/>
+      <c r="AN135" s="190"/>
+      <c r="AO135" s="190"/>
+      <c r="AP135" s="190"/>
+      <c r="AQ135" s="190"/>
+      <c r="AR135" s="191"/>
+      <c r="BB135" s="183"/>
+      <c r="BI135" s="189"/>
+      <c r="BJ135" s="190"/>
+      <c r="BK135" s="190"/>
+      <c r="BL135" s="190"/>
+      <c r="BM135" s="190"/>
+      <c r="BN135" s="190"/>
+      <c r="BO135" s="190"/>
+      <c r="BP135" s="190"/>
+      <c r="BQ135" s="190"/>
+      <c r="BR135" s="190"/>
+      <c r="BS135" s="191"/>
+      <c r="BX135" s="183"/>
       <c r="CY135" s="206" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="136" spans="5:107" ht="20.100000000000001" customHeight="1">
       <c r="AA136" s="143"/>
-      <c r="AH136" s="196"/>
-      <c r="AI136" s="197"/>
-      <c r="AJ136" s="197"/>
-      <c r="AK136" s="197"/>
-      <c r="AL136" s="197"/>
-      <c r="AM136" s="197"/>
-      <c r="AN136" s="197"/>
-      <c r="AO136" s="197"/>
-      <c r="AP136" s="197"/>
-      <c r="AQ136" s="197"/>
-      <c r="AR136" s="198"/>
-      <c r="BB136" s="184"/>
-      <c r="BI136" s="196"/>
-      <c r="BJ136" s="197"/>
-      <c r="BK136" s="197"/>
-      <c r="BL136" s="197"/>
-      <c r="BM136" s="197"/>
-      <c r="BN136" s="197"/>
-      <c r="BO136" s="197"/>
-      <c r="BP136" s="197"/>
-      <c r="BQ136" s="197"/>
-      <c r="BR136" s="197"/>
-      <c r="BS136" s="198"/>
-      <c r="BX136" s="184"/>
+      <c r="AH136" s="195"/>
+      <c r="AI136" s="196"/>
+      <c r="AJ136" s="196"/>
+      <c r="AK136" s="196"/>
+      <c r="AL136" s="196"/>
+      <c r="AM136" s="196"/>
+      <c r="AN136" s="196"/>
+      <c r="AO136" s="196"/>
+      <c r="AP136" s="196"/>
+      <c r="AQ136" s="196"/>
+      <c r="AR136" s="197"/>
+      <c r="BB136" s="183"/>
+      <c r="BI136" s="195"/>
+      <c r="BJ136" s="196"/>
+      <c r="BK136" s="196"/>
+      <c r="BL136" s="196"/>
+      <c r="BM136" s="196"/>
+      <c r="BN136" s="196"/>
+      <c r="BO136" s="196"/>
+      <c r="BP136" s="196"/>
+      <c r="BQ136" s="196"/>
+      <c r="BR136" s="196"/>
+      <c r="BS136" s="197"/>
+      <c r="BX136" s="183"/>
       <c r="CY136" s="207" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="137" spans="5:107" ht="20.100000000000001" customHeight="1">
       <c r="AA137" s="143"/>
-      <c r="BB137" s="184"/>
-      <c r="BX137" s="184"/>
+      <c r="BB137" s="183"/>
+      <c r="BX137" s="183"/>
     </row>
     <row r="138" spans="5:107" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="AA138" s="143"/>
-      <c r="BB138" s="184"/>
-      <c r="BX138" s="184"/>
+      <c r="BB138" s="183"/>
+      <c r="BX138" s="183"/>
     </row>
     <row r="139" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="AA139" s="261"/>
@@ -18590,7 +18454,7 @@
     <row r="140" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="CR140" s="274"/>
       <c r="CT140" s="275">
-        <v>724</v>
+        <v>159</v>
       </c>
       <c r="CU140" s="276"/>
       <c r="CV140" s="276"/>
@@ -18632,7 +18496,7 @@
       <c r="CK141" s="280"/>
       <c r="CR141" s="274"/>
       <c r="CT141" s="281">
-        <v>1399.7</v>
+        <v>327.2</v>
       </c>
       <c r="CU141" s="282"/>
       <c r="CV141" s="282"/>
@@ -18645,48 +18509,48 @@
     </row>
     <row r="142" spans="5:107" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1">
       <c r="K142" s="284">
-        <v>178</v>
+        <v>36</v>
       </c>
       <c r="L142" s="285"/>
       <c r="M142" s="285"/>
       <c r="N142" s="285"/>
       <c r="O142" s="286"/>
       <c r="P142" s="1">
-        <v>178</v>
+        <v>36</v>
       </c>
       <c r="AM142" s="284">
-        <v>247</v>
+        <v>17</v>
       </c>
       <c r="AN142" s="285"/>
       <c r="AO142" s="285"/>
       <c r="AP142" s="285"/>
       <c r="AQ142" s="286"/>
       <c r="AR142" s="1">
-        <v>247</v>
+        <v>17</v>
       </c>
       <c r="BL142" s="284">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="BM142" s="285"/>
       <c r="BN142" s="285"/>
       <c r="BO142" s="285"/>
       <c r="BP142" s="286"/>
       <c r="BQ142" s="1">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="CG142" s="284">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="CH142" s="285"/>
       <c r="CI142" s="285"/>
       <c r="CJ142" s="285"/>
       <c r="CK142" s="286"/>
       <c r="CL142" s="1">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="CR142" s="287"/>
       <c r="CT142" s="288">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="CU142" s="289"/>
       <c r="CV142" s="289"/>
@@ -18703,52 +18567,52 @@
       <c r="G143" s="292"/>
       <c r="H143" s="291"/>
       <c r="K143" s="293">
-        <v>446.1</v>
+        <v>48.9</v>
       </c>
       <c r="L143" s="294"/>
       <c r="M143" s="294"/>
       <c r="N143" s="294"/>
       <c r="O143" s="295"/>
       <c r="P143" s="1">
-        <v>446.1</v>
+        <v>48.9</v>
       </c>
       <c r="V143" s="291"/>
       <c r="W143" s="291"/>
       <c r="X143" s="291"/>
       <c r="Y143" s="291"/>
       <c r="AM143" s="293">
-        <v>770.8</v>
+        <v>94.3</v>
       </c>
       <c r="AN143" s="294"/>
       <c r="AO143" s="294"/>
       <c r="AP143" s="294"/>
       <c r="AQ143" s="295"/>
       <c r="AR143" s="1">
-        <v>770.8</v>
+        <v>94.3</v>
       </c>
       <c r="BL143" s="293">
-        <v>158.19999999999999</v>
+        <v>168.39999999999998</v>
       </c>
       <c r="BM143" s="294"/>
       <c r="BN143" s="294"/>
       <c r="BO143" s="294"/>
       <c r="BP143" s="295"/>
       <c r="BQ143" s="1">
-        <v>158.19999999999999</v>
+        <v>168.39999999999998</v>
       </c>
       <c r="CG143" s="293">
-        <v>24.6</v>
+        <v>15.6</v>
       </c>
       <c r="CH143" s="294"/>
       <c r="CI143" s="294"/>
       <c r="CJ143" s="294"/>
       <c r="CK143" s="295"/>
       <c r="CL143" s="1">
-        <v>24.6</v>
+        <v>15.6</v>
       </c>
       <c r="CR143" s="287"/>
       <c r="CT143" s="281">
-        <v>542.29999999999995</v>
+        <v>72.3</v>
       </c>
       <c r="CU143" s="282"/>
       <c r="CV143" s="282"/>
@@ -18806,7 +18670,8 @@
       <c r="Y145" s="291"/>
     </row>
   </sheetData>
-  <mergeCells count="532">
+  <dataConsolidate/>
+  <mergeCells count="535">
     <mergeCell ref="K142:O142"/>
     <mergeCell ref="AM142:AQ142"/>
     <mergeCell ref="BL142:BP142"/>
@@ -18841,7 +18706,6 @@
     <mergeCell ref="AD107:AG107"/>
     <mergeCell ref="AV107:AY107"/>
     <mergeCell ref="CY107:DB107"/>
-    <mergeCell ref="CY88:DB88"/>
     <mergeCell ref="J92:P93"/>
     <mergeCell ref="T92:Z92"/>
     <mergeCell ref="AA92:AK92"/>
@@ -18849,39 +18713,43 @@
     <mergeCell ref="BH95:BN97"/>
     <mergeCell ref="CY96:DB96"/>
     <mergeCell ref="CY97:DB97"/>
-    <mergeCell ref="CY79:DB79"/>
     <mergeCell ref="J83:N83"/>
     <mergeCell ref="CY83:DB83"/>
     <mergeCell ref="DC83:DE83"/>
     <mergeCell ref="AO87:AV87"/>
     <mergeCell ref="CY87:DB87"/>
-    <mergeCell ref="CY70:DB70"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="J74:N74"/>
+    <mergeCell ref="CY88:DB88"/>
     <mergeCell ref="AF76:AN77"/>
     <mergeCell ref="AO76:AV76"/>
     <mergeCell ref="BH77:BX78"/>
     <mergeCell ref="BY77:CA78"/>
     <mergeCell ref="CY78:DB78"/>
-    <mergeCell ref="J65:N65"/>
-    <mergeCell ref="CY65:DB65"/>
+    <mergeCell ref="CY79:DB79"/>
     <mergeCell ref="DC65:DE65"/>
     <mergeCell ref="AN68:AV68"/>
     <mergeCell ref="BY68:CJ69"/>
     <mergeCell ref="CY69:DB69"/>
-    <mergeCell ref="CA50:CD50"/>
-    <mergeCell ref="CG50:CR51"/>
-    <mergeCell ref="CY50:DB50"/>
+    <mergeCell ref="CY70:DB70"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="J74:N74"/>
     <mergeCell ref="J56:N56"/>
     <mergeCell ref="CY58:DB58"/>
     <mergeCell ref="AL59:AV60"/>
     <mergeCell ref="CY59:DB59"/>
+    <mergeCell ref="J65:N65"/>
+    <mergeCell ref="CY65:DB65"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="CA49:CD49"/>
+    <mergeCell ref="CY49:DB49"/>
+    <mergeCell ref="CA50:CD50"/>
+    <mergeCell ref="CG50:CR51"/>
+    <mergeCell ref="CY50:DB50"/>
     <mergeCell ref="H43:K43"/>
     <mergeCell ref="AE43:AG43"/>
     <mergeCell ref="AE44:AG44"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="CA49:CD49"/>
-    <mergeCell ref="CY49:DB49"/>
+    <mergeCell ref="BD45:BF45"/>
+    <mergeCell ref="BG45:BI45"/>
+    <mergeCell ref="BO45:BQ45"/>
     <mergeCell ref="P41:S41"/>
     <mergeCell ref="BF41:BI41"/>
     <mergeCell ref="BP41:BS41"/>
@@ -19347,14 +19215,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E7B308-EDD1-472D-8B99-595B81A497D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4793895-1760-4B21-96BC-04D52DEE1F31}">
   <sheetPr codeName="Sheet7">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:Z48"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>